<commit_message>
Updates on the data
</commit_message>
<xml_diff>
--- a/src/doc/acl/acl_configuration.xlsx
+++ b/src/doc/acl/acl_configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="573" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="To be filled up by developer" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="66">
   <si>
     <t>Menu Name</t>
   </si>
@@ -339,8 +339,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -452,7 +456,7 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -488,6 +492,8 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -523,6 +529,8 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -854,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -920,6 +928,9 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
       <c r="G3" s="15">
         <v>40909</v>
       </c>
@@ -931,6 +942,9 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
       <c r="G4" s="15">
         <v>40909</v>
       </c>
@@ -942,6 +956,9 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
       <c r="G5" s="15">
         <v>40909</v>
       </c>
@@ -952,6 +969,9 @@
       </c>
       <c r="D6" t="s">
         <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>65</v>
       </c>
       <c r="G6" s="15">
         <v>40909</v>
@@ -973,7 +993,7 @@
   <dimension ref="A1:K192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2853,7 +2873,7 @@
   <dimension ref="A1:L192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4776,10 +4796,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K192"/>
+  <dimension ref="A1:K190"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4872,6 +4892,9 @@
       <c r="A4" s="6">
         <v>1</v>
       </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
       <c r="C4" s="6">
         <v>3</v>
       </c>
@@ -4892,18 +4915,20 @@
       </c>
       <c r="I4" s="6" t="str">
         <f>CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A4),"''",SUBSTITUTE(A4,"'", "''") ), "'"&amp;SUBSTITUTE(A4,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B4),"''",SUBSTITUTE(B4,"'","''") ), "'"&amp;SUBSTITUTE(B4,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C4),"''",SUBSTITUTE(C4,"'","''") ), "'"&amp;SUBSTITUTE(C4,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D4),"''",SUBSTITUTE(D4,"'","''") ), "'"&amp;SUBSTITUTE(D4,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E4),"''",SUBSTITUTE(E4,"'","''") ), "'"&amp;SUBSTITUTE(E4,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F4),"''",SUBSTITUTE(F4,"'","''") ), "'"&amp;SUBSTITUTE(F4,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G4),"''",SUBSTITUTE(G4,"'","''") ), "'"&amp;SUBSTITUTE(G4,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H4),"''",SUBSTITUTE(H4,"'","''") ), "'"&amp;SUBSTITUTE(H4,"'","''")&amp;"'" ),");")</f>
-        <v>1,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>1,1,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J4" s="6" t="str">
         <f>IF($C$1="","", CONCATENATE($C$1,I4))</f>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (1,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (1,1,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="12">
         <v>2</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="12">
+        <v>3</v>
+      </c>
       <c r="C5" s="12">
         <v>3</v>
       </c>
@@ -4923,19 +4948,21 @@
         <v>1</v>
       </c>
       <c r="I5" s="6" t="str">
-        <f t="shared" ref="I5:I19" si="0">CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A5),"''",SUBSTITUTE(A5,"'", "''") ), "'"&amp;SUBSTITUTE(A5,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B5),"''",SUBSTITUTE(B5,"'","''") ), "'"&amp;SUBSTITUTE(B5,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C5),"''",SUBSTITUTE(C5,"'","''") ), "'"&amp;SUBSTITUTE(C5,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D5),"''",SUBSTITUTE(D5,"'","''") ), "'"&amp;SUBSTITUTE(D5,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E5),"''",SUBSTITUTE(E5,"'","''") ), "'"&amp;SUBSTITUTE(E5,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F5),"''",SUBSTITUTE(F5,"'","''") ), "'"&amp;SUBSTITUTE(F5,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G5),"''",SUBSTITUTE(G5,"'","''") ), "'"&amp;SUBSTITUTE(G5,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H5),"''",SUBSTITUTE(H5,"'","''") ), "'"&amp;SUBSTITUTE(H5,"'","''")&amp;"'" ),");")</f>
-        <v>2,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <f t="shared" ref="I5:I17" si="0">CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A5),"''",SUBSTITUTE(A5,"'", "''") ), "'"&amp;SUBSTITUTE(A5,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B5),"''",SUBSTITUTE(B5,"'","''") ), "'"&amp;SUBSTITUTE(B5,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C5),"''",SUBSTITUTE(C5,"'","''") ), "'"&amp;SUBSTITUTE(C5,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D5),"''",SUBSTITUTE(D5,"'","''") ), "'"&amp;SUBSTITUTE(D5,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E5),"''",SUBSTITUTE(E5,"'","''") ), "'"&amp;SUBSTITUTE(E5,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F5),"''",SUBSTITUTE(F5,"'","''") ), "'"&amp;SUBSTITUTE(F5,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G5),"''",SUBSTITUTE(G5,"'","''") ), "'"&amp;SUBSTITUTE(G5,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H5),"''",SUBSTITUTE(H5,"'","''") ), "'"&amp;SUBSTITUTE(H5,"'","''")&amp;"'" ),");")</f>
+        <v>2,3,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J5" s="6" t="str">
-        <f t="shared" ref="J5:J19" si="1">IF($C$1="","", CONCATENATE($C$1,I5))</f>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (2,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <f t="shared" ref="J5:J17" si="1">IF($C$1="","", CONCATENATE($C$1,I5))</f>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (2,3,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="12">
         <v>3</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="12">
+        <v>5</v>
+      </c>
       <c r="C6" s="12">
         <v>3</v>
       </c>
@@ -4956,18 +4983,20 @@
       </c>
       <c r="I6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>3,5,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (3,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (3,5,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="12">
         <v>4</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="12">
+        <v>6</v>
+      </c>
       <c r="C7" s="12">
         <v>3</v>
       </c>
@@ -4988,18 +5017,20 @@
       </c>
       <c r="I7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>4,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>4,6,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (4,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (4,6,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="12">
         <v>5</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="12">
+        <v>7</v>
+      </c>
       <c r="C8" s="12">
         <v>3</v>
       </c>
@@ -5020,18 +5051,20 @@
       </c>
       <c r="I8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>5,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>5,7,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (5,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (5,7,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="12">
         <v>6</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="12">
+        <v>8</v>
+      </c>
       <c r="C9" s="12">
         <v>3</v>
       </c>
@@ -5052,18 +5085,20 @@
       </c>
       <c r="I9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>6,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>6,8,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (6,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (6,8,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="12">
         <v>7</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="12">
+        <v>9</v>
+      </c>
       <c r="C10" s="12">
         <v>3</v>
       </c>
@@ -5084,20 +5119,22 @@
       </c>
       <c r="I10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>7,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>7,9,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J10" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (7,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (7,9,3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="12">
         <v>8</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="12">
+        <v>1</v>
+      </c>
       <c r="C11" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>18</v>
@@ -5116,19 +5153,23 @@
       </c>
       <c r="I11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>8,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>8,1,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J11" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (8,'',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (8,1,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="12">
         <v>9</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="12">
+        <v>1</v>
+      </c>
       <c r="D12" s="11" t="s">
         <v>18</v>
       </c>
@@ -5146,19 +5187,23 @@
       </c>
       <c r="I12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>9,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>9,2,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J12" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (9,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (9,2,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="6">
         <v>10</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="12">
+        <v>4</v>
+      </c>
+      <c r="C13" s="12">
+        <v>1</v>
+      </c>
       <c r="D13" s="11" t="s">
         <v>18</v>
       </c>
@@ -5176,19 +5221,23 @@
       </c>
       <c r="I13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>10,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>10,4,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J13" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (10,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (10,4,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="12">
         <v>11</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="12">
+        <v>6</v>
+      </c>
+      <c r="C14" s="12">
+        <v>1</v>
+      </c>
       <c r="D14" s="11" t="s">
         <v>18</v>
       </c>
@@ -5206,19 +5255,23 @@
       </c>
       <c r="I14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>11,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>11,6,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (11,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (11,6,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="12">
         <v>12</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="B15" s="12">
+        <v>7</v>
+      </c>
+      <c r="C15" s="12">
+        <v>1</v>
+      </c>
       <c r="D15" s="11" t="s">
         <v>18</v>
       </c>
@@ -5236,19 +5289,23 @@
       </c>
       <c r="I15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>12,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>12,7,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (12,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (12,7,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="12">
         <v>13</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
+      <c r="B16" s="12">
+        <v>8</v>
+      </c>
+      <c r="C16" s="12">
+        <v>1</v>
+      </c>
       <c r="D16" s="11" t="s">
         <v>18</v>
       </c>
@@ -5266,19 +5323,23 @@
       </c>
       <c r="I16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>13,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>13,8,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (13,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (13,8,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="12">
         <v>14</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
+      <c r="B17" s="12">
+        <v>9</v>
+      </c>
+      <c r="C17" s="12">
+        <v>1</v>
+      </c>
       <c r="D17" s="11" t="s">
         <v>18</v>
       </c>
@@ -5296,72 +5357,26 @@
       </c>
       <c r="I17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>14,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>14,9,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J17" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (14,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (14,9,1,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="12">
-        <v>15</v>
-      </c>
+      <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
-      <c r="D18" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="11">
-        <v>1</v>
-      </c>
-      <c r="I18" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>15,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
-      </c>
-      <c r="J18" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (15,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
-      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="12">
-        <v>16</v>
-      </c>
+      <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
-      <c r="D19" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" s="14">
-        <v>1</v>
-      </c>
-      <c r="I19" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>16,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
-      </c>
-      <c r="J19" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (16,'','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
-      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="12"/>
@@ -5930,7 +5945,7 @@
       <c r="D100" s="12"/>
       <c r="E100" s="12"/>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" s="13" customFormat="1">
       <c r="A101" s="12"/>
       <c r="B101" s="12"/>
       <c r="C101" s="12"/>
@@ -5944,7 +5959,7 @@
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
     </row>
-    <row r="103" spans="1:5" s="13" customFormat="1">
+    <row r="103" spans="1:5">
       <c r="A103" s="12"/>
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
@@ -6559,20 +6574,6 @@
       <c r="C190" s="12"/>
       <c r="D190" s="12"/>
       <c r="E190" s="12"/>
-    </row>
-    <row r="191" spans="1:5">
-      <c r="A191" s="12"/>
-      <c r="B191" s="12"/>
-      <c r="C191" s="12"/>
-      <c r="D191" s="12"/>
-      <c r="E191" s="12"/>
-    </row>
-    <row r="192" spans="1:5">
-      <c r="A192" s="12"/>
-      <c r="B192" s="12"/>
-      <c r="C192" s="12"/>
-      <c r="D192" s="12"/>
-      <c r="E192" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6590,7 +6591,7 @@
   <dimension ref="A1:K180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updated the data for TB_PERMISSION.
</commit_message>
<xml_diff>
--- a/src/doc/acl/acl_configuration.xlsx
+++ b/src/doc/acl/acl_configuration.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="68">
   <si>
     <t>Menu Name</t>
   </si>
@@ -222,6 +222,12 @@
   <si>
     <t>Peishan</t>
   </si>
+  <si>
+    <t>Search Projects (Volunteer)</t>
+  </si>
+  <si>
+    <t>/VMS/admin/volunteer/searchProjects.html</t>
+  </si>
 </sst>
 </file>
 
@@ -339,8 +345,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -484,7 +528,7 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="141">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -536,6 +580,25 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -587,6 +650,25 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1049,7 +1131,7 @@
   <dimension ref="A1:L195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1076,8 +1158,8 @@
         <v>46</v>
       </c>
       <c r="C1" s="6" t="str">
-        <f>CONCATENATE("INSERT INTO ",$B$1," (",$A$2,", ",$B$2,", ",$C$2,", ",$E$2,", ",$F$2,", ",$G$2,", ",$H$2,", ",$I$2,") VALUES (")</f>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (</v>
+        <f>CONCATENATE("INSERT INTO ",$B$1," (",$A$2,", ",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,", ",$H$2,", ",$I$2,") VALUES (")</f>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="5" customFormat="1">
@@ -1167,12 +1249,12 @@
         <v>1</v>
       </c>
       <c r="J4" s="6" t="str">
-        <f>CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A4),"''",SUBSTITUTE(A4,"'", "''") ), "'"&amp;SUBSTITUTE(A4,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B4),"''",SUBSTITUTE(B4,"'","''") ), "'"&amp;SUBSTITUTE(B4,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C4),"''",SUBSTITUTE(C4,"'","''") ), "'"&amp;SUBSTITUTE(C4,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E4),"''",SUBSTITUTE(E4,"'","''") ), "'"&amp;SUBSTITUTE(E4,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F4),"''",SUBSTITUTE(F4,"'","''") ), "'"&amp;SUBSTITUTE(F4,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G4),"''",SUBSTITUTE(G4,"'","''") ), "'"&amp;SUBSTITUTE(G4,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H4),"''",SUBSTITUTE(H4,"'","''") ), "'"&amp;SUBSTITUTE(H4,"'","''")&amp;"'" ),",",IF( ISTEXT($I$3), IF( ISBLANK(I4),"''",SUBSTITUTE(I4,"'","''") ), "'"&amp;SUBSTITUTE(I4,"'","''")&amp;"'" ),");")</f>
-        <v>1,'/VMS/common/welcome.html','Welcome page','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <f>CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A4),"''",SUBSTITUTE(A4,"'", "''") ), "'"&amp;SUBSTITUTE(A4,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B4),"''",SUBSTITUTE(B4,"'","''") ), "'"&amp;SUBSTITUTE(B4,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C4),"''",SUBSTITUTE(C4,"'","''") ), "'"&amp;SUBSTITUTE(C4,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D4),"''",SUBSTITUTE(D4,"'","''") ), "'"&amp;SUBSTITUTE(D4,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E4),"''",SUBSTITUTE(E4,"'","''") ), "'"&amp;SUBSTITUTE(E4,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F4),"''",SUBSTITUTE(F4,"'","''") ), "'"&amp;SUBSTITUTE(F4,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G4),"''",SUBSTITUTE(G4,"'","''") ), "'"&amp;SUBSTITUTE(G4,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H4),"''",SUBSTITUTE(H4,"'","''") ), "'"&amp;SUBSTITUTE(H4,"'","''")&amp;"'" ),",",IF( ISTEXT($I$3), IF( ISBLANK(I4),"''",SUBSTITUTE(I4,"'","''") ), "'"&amp;SUBSTITUTE(I4,"'","''")&amp;"'" ),");")</f>
+        <v>1,'/VMS/common/welcome.html','Welcome page','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K4" s="6" t="str">
         <f>IF($C$1="","", CONCATENATE($C$1,J4))</f>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (1,'/VMS/common/welcome.html','Welcome page','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (1,'/VMS/common/welcome.html','Welcome page','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1204,12 +1286,12 @@
         <v>1</v>
       </c>
       <c r="J5" s="6" t="str">
-        <f t="shared" ref="J5:J20" si="0">CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A5),"''",SUBSTITUTE(A5,"'", "''") ), "'"&amp;SUBSTITUTE(A5,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B5),"''",SUBSTITUTE(B5,"'","''") ), "'"&amp;SUBSTITUTE(B5,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C5),"''",SUBSTITUTE(C5,"'","''") ), "'"&amp;SUBSTITUTE(C5,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E5),"''",SUBSTITUTE(E5,"'","''") ), "'"&amp;SUBSTITUTE(E5,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F5),"''",SUBSTITUTE(F5,"'","''") ), "'"&amp;SUBSTITUTE(F5,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G5),"''",SUBSTITUTE(G5,"'","''") ), "'"&amp;SUBSTITUTE(G5,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H5),"''",SUBSTITUTE(H5,"'","''") ), "'"&amp;SUBSTITUTE(H5,"'","''")&amp;"'" ),",",IF( ISTEXT($I$3), IF( ISBLANK(I5),"''",SUBSTITUTE(I5,"'","''") ), "'"&amp;SUBSTITUTE(I5,"'","''")&amp;"'" ),");")</f>
-        <v>2,'/VMS/common/welcome.html','Manage Projects','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <f t="shared" ref="J5:J20" si="0">CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A5),"''",SUBSTITUTE(A5,"'", "''") ), "'"&amp;SUBSTITUTE(A5,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B5),"''",SUBSTITUTE(B5,"'","''") ), "'"&amp;SUBSTITUTE(B5,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C5),"''",SUBSTITUTE(C5,"'","''") ), "'"&amp;SUBSTITUTE(C5,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D5),"''",SUBSTITUTE(D5,"'","''") ), "'"&amp;SUBSTITUTE(D5,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E5),"''",SUBSTITUTE(E5,"'","''") ), "'"&amp;SUBSTITUTE(E5,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F5),"''",SUBSTITUTE(F5,"'","''") ), "'"&amp;SUBSTITUTE(F5,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G5),"''",SUBSTITUTE(G5,"'","''") ), "'"&amp;SUBSTITUTE(G5,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H5),"''",SUBSTITUTE(H5,"'","''") ), "'"&amp;SUBSTITUTE(H5,"'","''")&amp;"'" ),",",IF( ISTEXT($I$3), IF( ISBLANK(I5),"''",SUBSTITUTE(I5,"'","''") ), "'"&amp;SUBSTITUTE(I5,"'","''")&amp;"'" ),");")</f>
+        <v>2,'/VMS/common/welcome.html','Manage Projects',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K5" s="6" t="str">
-        <f t="shared" ref="K5:K20" si="1">IF($C$1="","", CONCATENATE($C$1,J5))</f>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (2,'/VMS/common/welcome.html','Manage Projects','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <f t="shared" ref="K5:K21" si="1">IF($C$1="","", CONCATENATE($C$1,J5))</f>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (2,'/VMS/common/welcome.html','Manage Projects',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1242,11 +1324,11 @@
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3,'/VMS/common/welcome.html','My Project Interests','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>3,'/VMS/common/welcome.html','My Project Interests',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K6" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (3,'/VMS/common/welcome.html','My Project Interests','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (3,'/VMS/common/welcome.html','My Project Interests',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1279,11 +1361,11 @@
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>4,'/VMS/common/welcome.html','Review Project Feedback','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>4,'/VMS/common/welcome.html','Review Project Feedback',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K7" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (4,'/VMS/common/welcome.html','Review Project Feedback','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (4,'/VMS/common/welcome.html','Review Project Feedback',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1316,11 +1398,11 @@
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>5,'/VMS/admin/volunteer/browseProject.html','Browse Project (Volunteer)','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>5,'/VMS/admin/volunteer/browseProject.html','Browse Project (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K8" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (5,'/VMS/admin/volunteer/browseProject.html','Browse Project (Volunteer)','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (5,'/VMS/admin/volunteer/browseProject.html','Browse Project (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1353,11 +1435,11 @@
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>6,'/VMS/admin/volunteer/viewProjectDetails.html','View Project Details (Volunteer)','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>6,'/VMS/admin/volunteer/viewProjectDetails.html','View Project Details (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K9" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (6,'/VMS/admin/volunteer/viewProjectDetails.html','View Project Details (Volunteer)','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (6,'/VMS/admin/volunteer/viewProjectDetails.html','View Project Details (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1390,11 +1472,11 @@
       </c>
       <c r="J10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>7,'/VMS/admin/volunteer/requestCertificate.html','Request Certificate (Volunteer)','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>7,'/VMS/admin/volunteer/requestCertificate.html','Request Certificate (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K10" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (7,'/VMS/admin/volunteer/requestCertificate.html','Request Certificate (Volunteer)','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (7,'/VMS/admin/volunteer/requestCertificate.html','Request Certificate (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1427,11 +1509,11 @@
       </c>
       <c r="J11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>8,'/VMS/admin/volunteer/raiseInterest.html','Raise Interest (Volunteer)','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>8,'/VMS/admin/volunteer/raiseInterest.html','Raise Interest (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K11" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (8,'/VMS/admin/volunteer/raiseInterest.html','Raise Interest (Volunteer)','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (8,'/VMS/admin/volunteer/raiseInterest.html','Raise Interest (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1464,11 +1546,11 @@
       </c>
       <c r="J12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>9,'/VMS/admin/volunteer/postExperienceAndFb.html','Post Experience and Feedback (Volunteer)','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>9,'/VMS/admin/volunteer/postExperienceAndFb.html','Post Experience and Feedback (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K12" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (9,'/VMS/admin/volunteer/postExperienceAndFb.html','Post Experience and Feedback (Volunteer)','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (9,'/VMS/admin/volunteer/postExperienceAndFb.html','Post Experience and Feedback (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1501,11 +1583,11 @@
       </c>
       <c r="J13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>10,'/VMS/common/welcome.html','My Profile','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>10,'/VMS/common/welcome.html','My Profile',7,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K13" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (10,'/VMS/common/welcome.html','My Profile','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (10,'/VMS/common/welcome.html','My Profile',7,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1538,11 +1620,11 @@
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>11,'/VMS/common/welcome.html','Change Password','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>11,'/VMS/common/welcome.html','Change Password',8,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K14" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (11,'/VMS/common/welcome.html','Change Password','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (11,'/VMS/common/welcome.html','Change Password',8,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1575,11 +1657,11 @@
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>12,'/VMS/common/welcome.html','Reset Password','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>12,'/VMS/common/welcome.html','Reset Password',9,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K15" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (12,'/VMS/common/welcome.html','Reset Password','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (12,'/VMS/common/welcome.html','Reset Password',9,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1612,11 +1694,11 @@
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>13,'/VMS/common/welcome.html','Manage Volunteer','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>13,'/VMS/common/welcome.html','Manage Volunteer',10,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K16" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (13,'/VMS/common/welcome.html','Manage Volunteer','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (13,'/VMS/common/welcome.html','Manage Volunteer',10,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1649,11 +1731,11 @@
       </c>
       <c r="J17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>14,'/VMS/common/welcome.html','Manage Staff','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>14,'/VMS/common/welcome.html','Manage Staff',11,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K17" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (14,'/VMS/common/welcome.html','Manage Staff','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (14,'/VMS/common/welcome.html','Manage Staff',11,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1686,11 +1768,11 @@
       </c>
       <c r="J18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>15,'/VMS/common/welcome.html','Generate Certificate','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>15,'/VMS/common/welcome.html','Generate Certificate',13,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K18" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (15,'/VMS/common/welcome.html','Generate Certificate','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (15,'/VMS/common/welcome.html','Generate Certificate',13,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1723,11 +1805,11 @@
       </c>
       <c r="J19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>16,'/VMS/common/welcome.html','Prepare Itinerary Plan','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>16,'/VMS/common/welcome.html','Prepare Itinerary Plan',14,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K19" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (16,'/VMS/common/welcome.html','Prepare Itinerary Plan','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (16,'/VMS/common/welcome.html','Prepare Itinerary Plan',14,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1760,20 +1842,49 @@
       </c>
       <c r="J20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>17,'/VMS/common/welcome.html','Review Intinerary Plan','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>17,'/VMS/common/welcome.html','Review Intinerary Plan',15,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K20" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (17,'/VMS/common/welcome.html','Review Intinerary Plan','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (17,'/VMS/common/welcome.html','Review Intinerary Plan',15,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="D21" s="12"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+      <c r="A21" s="12">
+        <v>18</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="6">
+        <v>5</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I21" s="11">
+        <v>1</v>
+      </c>
+      <c r="J21" s="6" t="str">
+        <f t="shared" ref="J21" si="2">CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A21),"''",SUBSTITUTE(A21,"'", "''") ), "'"&amp;SUBSTITUTE(A21,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B21),"''",SUBSTITUTE(B21,"'","''") ), "'"&amp;SUBSTITUTE(B21,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C21),"''",SUBSTITUTE(C21,"'","''") ), "'"&amp;SUBSTITUTE(C21,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D21),"''",SUBSTITUTE(D21,"'","''") ), "'"&amp;SUBSTITUTE(D21,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E21),"''",SUBSTITUTE(E21,"'","''") ), "'"&amp;SUBSTITUTE(E21,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F21),"''",SUBSTITUTE(F21,"'","''") ), "'"&amp;SUBSTITUTE(F21,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G21),"''",SUBSTITUTE(G21,"'","''") ), "'"&amp;SUBSTITUTE(G21,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H21),"''",SUBSTITUTE(H21,"'","''") ), "'"&amp;SUBSTITUTE(H21,"'","''")&amp;"'" ),",",IF( ISTEXT($I$3), IF( ISBLANK(I21),"''",SUBSTITUTE(I21,"'","''") ), "'"&amp;SUBSTITUTE(I21,"'","''")&amp;"'" ),");")</f>
+        <v>18,'/VMS/admin/volunteer/searchProjects.html','Search Projects (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K21" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (18,'/VMS/admin/volunteer/searchProjects.html','Search Projects (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
     </row>
     <row r="22" spans="1:11">
       <c r="D22" s="12"/>
@@ -3177,7 +3288,7 @@
   <dimension ref="A1:K192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5026,7 +5137,7 @@
   <dimension ref="A1:K190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Added the following URL to first tab. admin/volunteer/searchProjects.html
</commit_message>
<xml_diff>
--- a/src/doc/acl/acl_configuration.xlsx
+++ b/src/doc/acl/acl_configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="573" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="573"/>
   </bookViews>
   <sheets>
     <sheet name="To be filled up by developer" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="69">
   <si>
     <t>Menu Name</t>
   </si>
@@ -228,6 +228,9 @@
   <si>
     <t>/VMS/admin/volunteer/searchProjects.html</t>
   </si>
+  <si>
+    <t>admin/volunteer/searchProjects.html</t>
+  </si>
 </sst>
 </file>
 
@@ -345,8 +348,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="141">
+  <cellStyleXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -528,7 +537,7 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="141">
+  <cellStyles count="147">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -599,6 +608,9 @@
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -669,6 +681,9 @@
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -998,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1112,6 +1127,20 @@
         <v>65</v>
       </c>
       <c r="G6" s="15">
+        <v>40909</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="15">
         <v>40909</v>
       </c>
     </row>
@@ -1130,7 +1159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Feng Yan's URIs and Change Password
</commit_message>
<xml_diff>
--- a/src/doc/acl/acl_configuration.xlsx
+++ b/src/doc/acl/acl_configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="573"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="573" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To be filled up by developer" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="72">
   <si>
     <t>Menu Name</t>
   </si>
@@ -37,25 +37,10 @@
     <t>Link to menu?</t>
   </si>
   <si>
-    <t>admin/volunteer/browseProject.html</t>
-  </si>
-  <si>
     <t>✔</t>
   </si>
   <si>
     <t>Group</t>
-  </si>
-  <si>
-    <t>admin/volunteer/viewProjectDetails.html</t>
-  </si>
-  <si>
-    <t>admin/volunteer/requestCertificate.html</t>
-  </si>
-  <si>
-    <t>admin/volunteer/raiseInterest.html</t>
-  </si>
-  <si>
-    <t>admin/volunteer/postExperienceAndFb.html</t>
   </si>
   <si>
     <t>Parent Menu Name</t>
@@ -229,7 +214,31 @@
     <t>/VMS/admin/volunteer/searchProjects.html</t>
   </si>
   <si>
-    <t>admin/volunteer/searchProjects.html</t>
+    <t>Propose Project</t>
+  </si>
+  <si>
+    <t>/VMS/admin/volunteer/proposeNewProject.html</t>
+  </si>
+  <si>
+    <t>/VMS/admin/volunteer/browseProjectProposal.html</t>
+  </si>
+  <si>
+    <t>/VMS/admin/volunteer/searchProjectProposal.html</t>
+  </si>
+  <si>
+    <t>/VMS/admin/volunteer/viewProjectProposalDetails.html</t>
+  </si>
+  <si>
+    <t>/VMS/admin/volunteer/reviewProposal.html</t>
+  </si>
+  <si>
+    <t>/VMS/admin/user/changePassword.html</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -304,7 +313,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +338,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -348,7 +363,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="147">
+  <cellStyleXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -496,8 +511,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -536,8 +569,19 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="147">
+  <cellStyles count="165">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -611,6 +655,15 @@
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -684,6 +737,15 @@
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1013,30 +1075,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -1045,15 +1106,15 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1062,13 +1123,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G2" s="15">
         <v>40909</v>
@@ -1079,10 +1140,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G3" s="15">
         <v>40909</v>
@@ -1093,10 +1154,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G4" s="15">
         <v>40909</v>
@@ -1107,10 +1168,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G5" s="15">
         <v>40909</v>
@@ -1121,10 +1182,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G6" s="15">
         <v>40909</v>
@@ -1135,14 +1196,108 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G7" s="15">
         <v>40909</v>
       </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="15">
+        <v>40909</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="15">
+        <v>40910</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="15">
+        <v>40911</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="15">
+        <v>40912</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="15">
+        <v>40913</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="15">
+        <v>40909</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="E14" s="1"/>
+      <c r="G14" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1159,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L195"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1181,10 +1336,10 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C1" s="6" t="str">
         <f>CONCATENATE("INSERT INTO ",$B$1," (",$A$2,", ",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,", ",$H$2,", ",$I$2,") VALUES (")</f>
@@ -1193,63 +1348,63 @@
     </row>
     <row r="2" spans="1:12" s="5" customFormat="1">
       <c r="A2" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J3" s="10">
         <v>1</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1257,22 +1412,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I4" s="11">
         <v>1</v>
@@ -1291,25 +1446,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D5" s="6">
         <v>2</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I5" s="11">
         <v>1</v>
@@ -1328,25 +1483,25 @@
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D6" s="6">
         <v>3</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I6" s="11">
         <v>1</v>
@@ -1365,25 +1520,25 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D7" s="6">
         <v>4</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I7" s="11">
         <v>1</v>
@@ -1402,25 +1557,25 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>50</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>55</v>
       </c>
       <c r="D8" s="6">
         <v>5</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I8" s="11">
         <v>1</v>
@@ -1439,25 +1594,25 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D9" s="6">
         <v>5</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I9" s="11">
         <v>1</v>
@@ -1476,25 +1631,25 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D10" s="6">
         <v>5</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I10" s="11">
         <v>1</v>
@@ -1513,25 +1668,25 @@
         <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D11" s="6">
         <v>5</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I11" s="11">
         <v>1</v>
@@ -1550,25 +1705,25 @@
         <v>9</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D12" s="6">
         <v>5</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I12" s="11">
         <v>1</v>
@@ -1587,25 +1742,25 @@
         <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D13" s="6">
         <v>7</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I13" s="11">
         <v>1</v>
@@ -1623,37 +1778,37 @@
       <c r="A14" s="12">
         <v>11</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>49</v>
+      <c r="B14" t="s">
+        <v>69</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D14" s="6">
         <v>8</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I14" s="11">
         <v>1</v>
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>11,'/VMS/common/welcome.html','Change Password',8,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>11,'/VMS/admin/user/changePassword.html','Change Password',8,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K14" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (11,'/VMS/common/welcome.html','Change Password',8,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (11,'/VMS/admin/user/changePassword.html','Change Password',8,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1661,25 +1816,25 @@
         <v>12</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D15" s="6">
         <v>9</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I15" s="11">
         <v>1</v>
@@ -1698,25 +1853,25 @@
         <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D16" s="6">
         <v>10</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I16" s="11">
         <v>1</v>
@@ -1735,25 +1890,25 @@
         <v>14</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D17" s="6">
         <v>11</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I17" s="11">
         <v>1</v>
@@ -1772,25 +1927,25 @@
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D18" s="6">
         <v>13</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I18" s="11">
         <v>1</v>
@@ -1809,25 +1964,25 @@
         <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D19" s="6">
         <v>14</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I19" s="11">
         <v>1</v>
@@ -1846,25 +2001,25 @@
         <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D20" s="6">
         <v>15</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I20" s="11">
         <v>1</v>
@@ -1883,25 +2038,25 @@
         <v>18</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D21" s="6">
         <v>5</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I21" s="11">
         <v>1</v>
@@ -1915,13 +2070,42 @@
         <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (18,'/VMS/admin/volunteer/searchProjects.html','Search Projects (Volunteer)',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
-      <c r="D22" s="12"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+    <row r="22" spans="1:11" s="18" customFormat="1">
+      <c r="A22" s="16">
+        <v>19</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="18">
+        <v>17</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="19">
+        <v>1</v>
+      </c>
+      <c r="J22" s="18" t="str">
+        <f t="shared" ref="J22" si="3">CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A22),"''",SUBSTITUTE(A22,"'", "''") ), "'"&amp;SUBSTITUTE(A22,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B22),"''",SUBSTITUTE(B22,"'","''") ), "'"&amp;SUBSTITUTE(B22,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C22),"''",SUBSTITUTE(C22,"'","''") ), "'"&amp;SUBSTITUTE(C22,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D22),"''",SUBSTITUTE(D22,"'","''") ), "'"&amp;SUBSTITUTE(D22,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E22),"''",SUBSTITUTE(E22,"'","''") ), "'"&amp;SUBSTITUTE(E22,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F22),"''",SUBSTITUTE(F22,"'","''") ), "'"&amp;SUBSTITUTE(F22,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G22),"''",SUBSTITUTE(G22,"'","''") ), "'"&amp;SUBSTITUTE(G22,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H22),"''",SUBSTITUTE(H22,"'","''") ), "'"&amp;SUBSTITUTE(H22,"'","''")&amp;"'" ),",",IF( ISTEXT($I$3), IF( ISBLANK(I22),"''",SUBSTITUTE(I22,"'","''") ), "'"&amp;SUBSTITUTE(I22,"'","''")&amp;"'" ),");")</f>
+        <v>19,'/VMS/admin/volunteer/proposeNewProject.html','Propose Project',17,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K22" s="18" t="str">
+        <f t="shared" ref="K22" si="4">IF($C$1="","", CONCATENATE($C$1,J22))</f>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (19,'/VMS/admin/volunteer/proposeNewProject.html','Propose Project',17,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
     </row>
     <row r="23" spans="1:11">
       <c r="D23" s="12"/>
@@ -3317,7 +3501,7 @@
   <dimension ref="A1:K192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3337,10 +3521,10 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C1" s="6" t="str">
         <f>CONCATENATE("INSERT INTO ",$B$1," (",$A$2,", ",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,", ",$H$2,") VALUES (")</f>
@@ -3349,59 +3533,59 @@
     </row>
     <row r="2" spans="1:11" s="5" customFormat="1">
       <c r="A2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I3" s="10">
         <v>1</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3409,19 +3593,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H4" s="11">
         <v>1</v>
@@ -3443,19 +3627,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H5" s="14">
         <v>1</v>
@@ -3477,19 +3661,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H6" s="11">
         <v>1</v>
@@ -3511,19 +3695,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H7" s="14">
         <v>1</v>
@@ -3545,19 +3729,19 @@
         <v>1</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H8" s="11">
         <v>1</v>
@@ -3577,19 +3761,19 @@
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H9" s="14">
         <v>1</v>
@@ -3611,19 +3795,19 @@
         <v>6</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H10" s="11">
         <v>1</v>
@@ -3645,19 +3829,19 @@
         <v>6</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H11" s="14">
         <v>1</v>
@@ -3679,19 +3863,19 @@
         <v>6</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H12" s="11">
         <v>1</v>
@@ -3713,19 +3897,19 @@
         <v>6</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H13" s="14">
         <v>1</v>
@@ -3747,19 +3931,19 @@
         <v>6</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H14" s="11">
         <v>1</v>
@@ -3779,19 +3963,19 @@
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H15" s="14">
         <v>1</v>
@@ -3813,19 +3997,19 @@
         <v>12</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H16" s="11">
         <v>1</v>
@@ -3845,19 +4029,19 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H17" s="14">
         <v>1</v>
@@ -3879,19 +4063,19 @@
         <v>14</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H18" s="11">
         <v>1</v>
@@ -3913,19 +4097,19 @@
         <v>14</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H19" s="14">
         <v>1</v>
@@ -3939,12 +4123,39 @@
         <v>INSERT INTO TB_MENU_FUNCTION (MENU_FUNC_ID, PRNT_MENU_FUNC_ID, MENU_FUNC_NME, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (16,14,'Review Intinerary Plan','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
+    <row r="20" spans="1:10" s="18" customFormat="1">
+      <c r="A20" s="16">
+        <v>17</v>
+      </c>
+      <c r="B20" s="16">
+        <v>1</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="20">
+        <v>1</v>
+      </c>
+      <c r="I20" s="18" t="str">
+        <f t="shared" ref="I20" si="2">CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A20),"''",SUBSTITUTE(A20,"'", "''") ), "'"&amp;SUBSTITUTE(A20,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B20),"''",SUBSTITUTE(B20,"'","''") ), "'"&amp;SUBSTITUTE(B20,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C20),"''",SUBSTITUTE(C20,"'","''") ), "'"&amp;SUBSTITUTE(C20,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D20),"''",SUBSTITUTE(D20,"'","''") ), "'"&amp;SUBSTITUTE(D20,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E20),"''",SUBSTITUTE(E20,"'","''") ), "'"&amp;SUBSTITUTE(E20,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F20),"''",SUBSTITUTE(F20,"'","''") ), "'"&amp;SUBSTITUTE(F20,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G20),"''",SUBSTITUTE(G20,"'","''") ), "'"&amp;SUBSTITUTE(G20,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H20),"''",SUBSTITUTE(H20,"'","''") ), "'"&amp;SUBSTITUTE(H20,"'","''")&amp;"'" ),");")</f>
+        <v>17,1,'Propose Project','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="J20" s="18" t="str">
+        <f t="shared" ref="J20" si="3">IF($C$1="","", CONCATENATE($C$1,I20))</f>
+        <v>INSERT INTO TB_MENU_FUNCTION (MENU_FUNC_ID, PRNT_MENU_FUNC_ID, MENU_FUNC_NME, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (17,1,'Propose Project','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="12"/>
@@ -5166,7 +5377,7 @@
   <dimension ref="A1:K190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5186,10 +5397,10 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="C1" s="6" t="str">
         <f>CONCATENATE("INSERT INTO ",$B$1," (",$A$2,", ",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,", ",$H$2,") VALUES (")</f>
@@ -5198,61 +5409,61 @@
     </row>
     <row r="2" spans="1:11" s="5" customFormat="1">
       <c r="A2" s="7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I3" s="10">
         <v>1</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -5266,16 +5477,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H4" s="11">
         <v>1</v>
@@ -5300,16 +5511,16 @@
         <v>3</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H5" s="14">
         <v>1</v>
@@ -5334,16 +5545,16 @@
         <v>3</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H6" s="11">
         <v>1</v>
@@ -5368,16 +5579,16 @@
         <v>3</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H7" s="14">
         <v>1</v>
@@ -5402,16 +5613,16 @@
         <v>3</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H8" s="11">
         <v>1</v>
@@ -5436,16 +5647,16 @@
         <v>3</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H9" s="14">
         <v>1</v>
@@ -5470,16 +5681,16 @@
         <v>3</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H10" s="11">
         <v>1</v>
@@ -5504,16 +5715,16 @@
         <v>1</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H11" s="14">
         <v>1</v>
@@ -5538,16 +5749,16 @@
         <v>1</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H12" s="11">
         <v>1</v>
@@ -5572,16 +5783,16 @@
         <v>1</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H13" s="14">
         <v>1</v>
@@ -5606,16 +5817,16 @@
         <v>1</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H14" s="11">
         <v>1</v>
@@ -5640,16 +5851,16 @@
         <v>1</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H15" s="14">
         <v>1</v>
@@ -5674,16 +5885,16 @@
         <v>1</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H16" s="11">
         <v>1</v>
@@ -5708,16 +5919,16 @@
         <v>1</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H17" s="14">
         <v>1</v>
@@ -6978,10 +7189,10 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C1" s="6" t="str">
         <f>CONCATENATE("INSERT INTO ",$B$1," (",$A$2,", ",$B$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,", ",$H$2,") VALUES (")</f>
@@ -6990,57 +7201,57 @@
     </row>
     <row r="2" spans="1:11" s="5" customFormat="1">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I3" s="10">
         <v>1</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -7051,16 +7262,16 @@
         <v>38</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H4" s="11">
         <v>1</v>
@@ -7083,16 +7294,16 @@
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H5" s="11">
         <v>1</v>
@@ -7115,16 +7326,16 @@
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H6" s="11">
         <v>1</v>
@@ -7147,16 +7358,16 @@
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H7" s="11">
         <v>1</v>

</xml_diff>

<commit_message>
Updated the URL for My Project Interest
</commit_message>
<xml_diff>
--- a/src/doc/acl/acl_configuration.xlsx
+++ b/src/doc/acl/acl_configuration.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="573" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="573"/>
   </bookViews>
   <sheets>
     <sheet name="To be filled up by developer" sheetId="1" r:id="rId1"/>
     <sheet name="TB_MENU_FUNCTION" sheetId="3" r:id="rId2"/>
     <sheet name="TB_PERMISSION" sheetId="4" r:id="rId3"/>
-    <sheet name="TB_ROLE_FUNCTION" sheetId="2" r:id="rId4"/>
-    <sheet name="TB_ROLE" sheetId="5" r:id="rId5"/>
+    <sheet name="TB_PERMISSION BAK" sheetId="7" r:id="rId4"/>
+    <sheet name="TB_ROLE_FUNCTION" sheetId="2" r:id="rId5"/>
+    <sheet name="TB_ROLE" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="128">
   <si>
     <t>Menu Name</t>
   </si>
@@ -339,6 +340,75 @@
   <si>
     <t>Forget Password</t>
   </si>
+  <si>
+    <t>/VMS/project/updateProject.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/viewProject.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/browseProjectFeedback.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/viewProjectFeedbackDetails.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/approveFb.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/rejectFb.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/browseProjectProposal.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/searchProjectProposal.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/viewProjectProposalDetails.html</t>
+  </si>
+  <si>
+    <t>/VMS/volunteer/browseProject.html</t>
+  </si>
+  <si>
+    <t>/VMS/volunteer/searchProjects.html</t>
+  </si>
+  <si>
+    <t>/VMS/volunteer/viewProjectDetails.html</t>
+  </si>
+  <si>
+    <t>/VMS/volunteer/requestCertificate.html</t>
+  </si>
+  <si>
+    <t>/VMS/volunteer/postExperienceAndFb.html</t>
+  </si>
+  <si>
+    <t>/VMS/volunteer/raiseInterest.html</t>
+  </si>
+  <si>
+    <t>/VMS/volunteer/updateVolunteer.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/VMS/certificate/generateCertificate.html </t>
+  </si>
+  <si>
+    <t>/VMS/project/reviewProposal.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/proposeNewProject.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/listProjects.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/createProject.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/manageProjectMember.html</t>
+  </si>
+  <si>
+    <t>/VMS/project/viewProjectInterest.html</t>
+  </si>
 </sst>
 </file>
 
@@ -481,7 +551,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="435">
+  <cellStyleXfs count="443">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -917,8 +987,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -974,7 +1052,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -983,7 +1060,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="435">
+  <cellStyles count="443">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1201,6 +1278,10 @@
     <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1418,6 +1499,10 @@
     <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1749,9 +1834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2228,7 +2313,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="21" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="12" t="s">
@@ -2238,7 +2323,7 @@
         <v>22</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>43</v>
+        <v>127</v>
       </c>
       <c r="G22" t="s">
         <v>59</v>
@@ -2306,7 +2391,7 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>104</v>
       </c>
       <c r="C25" t="s">
@@ -2400,7 +2485,7 @@
   <dimension ref="A1:K186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4288,8 +4373,8 @@
   <dimension ref="A1:L207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4420,7 +4505,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>21</v>
@@ -4445,11 +4530,11 @@
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" ref="J5:J34" si="0">CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A5),"''",SUBSTITUTE(A5,"'", "''") ), "'"&amp;SUBSTITUTE(A5,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B5),"''",SUBSTITUTE(B5,"'","''") ), "'"&amp;SUBSTITUTE(B5,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C5),"''",SUBSTITUTE(C5,"'","''") ), "'"&amp;SUBSTITUTE(C5,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D5),"''",SUBSTITUTE(D5,"'","''") ), "'"&amp;SUBSTITUTE(D5,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E5),"''",SUBSTITUTE(E5,"'","''") ), "'"&amp;SUBSTITUTE(E5,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F5),"''",SUBSTITUTE(F5,"'","''") ), "'"&amp;SUBSTITUTE(F5,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G5),"''",SUBSTITUTE(G5,"'","''") ), "'"&amp;SUBSTITUTE(G5,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H5),"''",SUBSTITUTE(H5,"'","''") ), "'"&amp;SUBSTITUTE(H5,"'","''")&amp;"'" ),",",IF( ISTEXT($I$3), IF( ISBLANK(I5),"''",SUBSTITUTE(I5,"'","''") ), "'"&amp;SUBSTITUTE(I5,"'","''")&amp;"'" ),");")</f>
-        <v>2,'/VMS/admin/project/listProjects.html','Manage Projects',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>2,'/VMS/project/listProjects.html','Manage Projects',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K5" s="6" t="str">
         <f t="shared" ref="K5:K34" si="1">IF($C$1="","", CONCATENATE($C$1,J5))</f>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (2,'/VMS/admin/project/listProjects.html','Manage Projects',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (2,'/VMS/project/listProjects.html','Manage Projects',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -4457,7 +4542,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
         <v>86</v>
@@ -4482,11 +4567,11 @@
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3,'/VMS/admin/project/createProject.html','Create Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>3,'/VMS/project/createProject.html','Create Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K6" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (3,'/VMS/admin/project/createProject.html','Create Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (3,'/VMS/project/createProject.html','Create Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -4494,7 +4579,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="C7" t="s">
         <v>87</v>
@@ -4519,11 +4604,11 @@
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>4,'/VMS/admin/project/updateProject.html','Update Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>4,'/VMS/project/updateProject.html','Update Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K7" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (4,'/VMS/admin/project/updateProject.html','Update Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (4,'/VMS/project/updateProject.html','Update Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -4531,7 +4616,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
         <v>89</v>
@@ -4556,11 +4641,11 @@
       </c>
       <c r="J8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>5,'/VMS/admin/project/viewProject.html','View Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>5,'/VMS/project/viewProject.html','View Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K8" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (5,'/VMS/admin/project/viewProject.html','View Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (5,'/VMS/project/viewProject.html','View Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -4568,7 +4653,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
         <v>75</v>
@@ -4593,11 +4678,11 @@
       </c>
       <c r="J9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>6,'/VMS/admin/member/manageProjectMember.html','Manage Project Member',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>6,'/VMS/project/manageProjectMember.html','Manage Project Member',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K9" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (6,'/VMS/admin/member/manageProjectMember.html','Manage Project Member',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (6,'/VMS/project/manageProjectMember.html','Manage Project Member',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -4605,7 +4690,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
@@ -4630,11 +4715,11 @@
       </c>
       <c r="J10" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>7,'/VMS/admin/project/browseProjectFeedback.html','Review Project Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>7,'/VMS/project/browseProjectFeedback.html','Review Project Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K10" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (7,'/VMS/admin/project/browseProjectFeedback.html','Review Project Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (7,'/VMS/project/browseProjectFeedback.html','Review Project Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -4642,7 +4727,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C11" t="s">
         <v>100</v>
@@ -4667,11 +4752,11 @@
       </c>
       <c r="J11" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>8,'/VMS/admin/project/viewProjectFeedbackDetails.html','View Project Feeback Details',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>8,'/VMS/project/viewProjectFeedbackDetails.html','View Project Feeback Details',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K11" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (8,'/VMS/admin/project/viewProjectFeedbackDetails.html','View Project Feeback Details',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (8,'/VMS/project/viewProjectFeedbackDetails.html','View Project Feeback Details',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -4679,7 +4764,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
         <v>101</v>
@@ -4704,11 +4789,11 @@
       </c>
       <c r="J12" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>9,'/VMS/admin/project/approveFb.html','Approve Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>9,'/VMS/project/approveFb.html','Approve Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K12" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (9,'/VMS/admin/project/approveFb.html','Approve Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (9,'/VMS/project/approveFb.html','Approve Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -4716,7 +4801,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
         <v>102</v>
@@ -4741,11 +4826,11 @@
       </c>
       <c r="J13" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>10,'/VMS/admin/project/rejectFb.html','Reject Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>10,'/VMS/project/rejectFb.html','Reject Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K13" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (10,'/VMS/admin/project/rejectFb.html','Reject Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (10,'/VMS/project/rejectFb.html','Reject Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -4753,7 +4838,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="C14" t="s">
         <v>103</v>
@@ -4778,11 +4863,11 @@
       </c>
       <c r="J14" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>11,'/VMS/admin/volunteer/browseProjectProposal.html','Browse Project Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>11,'/VMS/project/browseProjectProposal.html','Browse Project Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K14" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (11,'/VMS/admin/volunteer/browseProjectProposal.html','Browse Project Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (11,'/VMS/project/browseProjectProposal.html','Browse Project Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -4790,7 +4875,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="C15" t="s">
         <v>90</v>
@@ -4815,11 +4900,11 @@
       </c>
       <c r="J15" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>12,'/VMS/admin/volunteer/searchProjectProposal.html','Search Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>12,'/VMS/project/searchProjectProposal.html','Search Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K15" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (12,'/VMS/admin/volunteer/searchProjectProposal.html','Search Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (12,'/VMS/project/searchProjectProposal.html','Search Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -4827,7 +4912,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="C16" t="s">
         <v>91</v>
@@ -4852,11 +4937,11 @@
       </c>
       <c r="J16" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>13,'/VMS/admin/volunteer/viewProjectProposalDetails.html','View Project Proposal Details',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>13,'/VMS/project/viewProjectProposalDetails.html','View Project Proposal Details',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K16" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (13,'/VMS/admin/volunteer/viewProjectProposalDetails.html','View Project Proposal Details',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (13,'/VMS/project/viewProjectProposalDetails.html','View Project Proposal Details',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -4864,7 +4949,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
         <v>92</v>
@@ -4889,11 +4974,11 @@
       </c>
       <c r="J17" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>14,'/VMS/admin/volunteer/reviewProposal.html','Review Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>14,'/VMS/project/reviewProposal.html','Review Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K17" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (14,'/VMS/admin/volunteer/reviewProposal.html','Review Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (14,'/VMS/project/reviewProposal.html','Review Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="20" customFormat="1">
@@ -4901,7 +4986,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>63</v>
+        <v>123</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>62</v>
@@ -4926,11 +5011,11 @@
       </c>
       <c r="J18" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>15,'/VMS/admin/volunteer/proposeNewProject.html','Propose Project',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>15,'/VMS/project/proposeNewProject.html','Propose Project',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K18" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (15,'/VMS/admin/volunteer/proposeNewProject.html','Propose Project',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (15,'/VMS/project/proposeNewProject.html','Propose Project',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -4938,7 +5023,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>49</v>
@@ -4963,11 +5048,11 @@
       </c>
       <c r="J19" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>16,'/VMS/admin/volunteer/browseProject.html','Browse Project (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>16,'/VMS/volunteer/browseProject.html','Browse Project (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K19" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (16,'/VMS/admin/volunteer/browseProject.html','Browse Project (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (16,'/VMS/volunteer/browseProject.html','Browse Project (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -4975,7 +5060,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>60</v>
@@ -5000,11 +5085,11 @@
       </c>
       <c r="J20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>17,'/VMS/admin/volunteer/searchProjects.html','Search Projects (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>17,'/VMS/volunteer/searchProjects.html','Search Projects (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K20" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (17,'/VMS/admin/volunteer/searchProjects.html','Search Projects (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (17,'/VMS/volunteer/searchProjects.html','Search Projects (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -5012,7 +5097,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>48</v>
@@ -5037,11 +5122,11 @@
       </c>
       <c r="J21" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>18,'/VMS/admin/volunteer/viewProjectDetails.html','View Project Details (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>18,'/VMS/volunteer/viewProjectDetails.html','View Project Details (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K21" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (18,'/VMS/admin/volunteer/viewProjectDetails.html','View Project Details (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (18,'/VMS/volunteer/viewProjectDetails.html','View Project Details (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -5049,7 +5134,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>47</v>
@@ -5074,11 +5159,11 @@
       </c>
       <c r="J22" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>19,'/VMS/admin/volunteer/requestCertificate.html','Request Certificate (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>19,'/VMS/volunteer/requestCertificate.html','Request Certificate (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K22" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (19,'/VMS/admin/volunteer/requestCertificate.html','Request Certificate (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (19,'/VMS/volunteer/requestCertificate.html','Request Certificate (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -5086,7 +5171,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>53</v>
@@ -5111,11 +5196,11 @@
       </c>
       <c r="J23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>20,'/VMS/admin/volunteer/postExperienceAndFb.html','Post Experience and Feedback (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>20,'/VMS/volunteer/postExperienceAndFb.html','Post Experience and Feedback (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K23" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (20,'/VMS/admin/volunteer/postExperienceAndFb.html','Post Experience and Feedback (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (20,'/VMS/volunteer/postExperienceAndFb.html','Post Experience and Feedback (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -5123,7 +5208,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>51</v>
@@ -5148,19 +5233,19 @@
       </c>
       <c r="J24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>21,'/VMS/admin/volunteer/raiseInterest.html','Raise Interest (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>21,'/VMS/volunteer/raiseInterest.html','Raise Interest (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K24" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (21,'/VMS/admin/volunteer/raiseInterest.html','Raise Interest (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (21,'/VMS/volunteer/raiseInterest.html','Raise Interest (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="6">
         <v>22</v>
       </c>
-      <c r="B25" s="27" t="s">
-        <v>43</v>
+      <c r="B25" s="20" t="s">
+        <v>127</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>22</v>
@@ -5185,11 +5270,11 @@
       </c>
       <c r="J25" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>22,'/VMS/common/welcome.html','My Project Interests',7,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>22,'/VMS/project/viewProjectInterest.html','My Project Interests',7,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K25" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (22,'/VMS/common/welcome.html','My Project Interests',7,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (22,'/VMS/project/viewProjectInterest.html','My Project Interests',7,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -5231,7 +5316,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>26</v>
@@ -5256,11 +5341,11 @@
       </c>
       <c r="J27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>24,'/VMS/common/volunteer/updateVolunteer.html','My Profile',9,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>24,'/VMS/volunteer/updateVolunteer.html','My Profile',9,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K27" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (24,'/VMS/common/volunteer/updateVolunteer.html','My Profile',9,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (24,'/VMS/volunteer/updateVolunteer.html','My Profile',9,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -5304,7 +5389,7 @@
       <c r="A29" s="6">
         <v>26</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>43</v>
       </c>
       <c r="C29" s="12" t="s">
@@ -5341,7 +5426,7 @@
       <c r="A30" s="12">
         <v>27</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="27" t="s">
         <v>43</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -5378,7 +5463,7 @@
       <c r="A31" s="6">
         <v>28</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="27" t="s">
         <v>43</v>
       </c>
       <c r="C31" s="12" t="s">
@@ -5416,7 +5501,7 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>31</v>
@@ -5441,18 +5526,18 @@
       </c>
       <c r="J32" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>29,'/VMS/admin/reports/generateCertificate.html ','Generate Certificate',16,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>29,'/VMS/certificate/generateCertificate.html ','Generate Certificate',16,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="K32" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (29,'/VMS/admin/reports/generateCertificate.html ','Generate Certificate',16,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (29,'/VMS/certificate/generateCertificate.html ','Generate Certificate',16,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="6">
         <v>30</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="27" t="s">
         <v>43</v>
       </c>
       <c r="C33" s="12" t="s">
@@ -5489,7 +5574,7 @@
       <c r="A34" s="6">
         <v>31</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="27" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="12" t="s">
@@ -6899,10 +6984,2624 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L207"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="9.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" style="6" customWidth="1"/>
+    <col min="12" max="16384" width="9.1640625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="6" t="str">
+        <f>CONCATENATE("INSERT INTO ",$B$1," (",$A$2,", ",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,", ",$H$2,", ",$I$2,") VALUES (")</f>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="5" customFormat="1">
+      <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" ht="16" thickBot="1">
+      <c r="A3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="10">
+        <v>1</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="11">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6" t="str">
+        <f>CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A4),"''",SUBSTITUTE(A4,"'", "''") ), "'"&amp;SUBSTITUTE(A4,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B4),"''",SUBSTITUTE(B4,"'","''") ), "'"&amp;SUBSTITUTE(B4,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C4),"''",SUBSTITUTE(C4,"'","''") ), "'"&amp;SUBSTITUTE(C4,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D4),"''",SUBSTITUTE(D4,"'","''") ), "'"&amp;SUBSTITUTE(D4,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E4),"''",SUBSTITUTE(E4,"'","''") ), "'"&amp;SUBSTITUTE(E4,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F4),"''",SUBSTITUTE(F4,"'","''") ), "'"&amp;SUBSTITUTE(F4,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G4),"''",SUBSTITUTE(G4,"'","''") ), "'"&amp;SUBSTITUTE(G4,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H4),"''",SUBSTITUTE(H4,"'","''") ), "'"&amp;SUBSTITUTE(H4,"'","''")&amp;"'" ),",",IF( ISTEXT($I$3), IF( ISBLANK(I4),"''",SUBSTITUTE(I4,"'","''") ), "'"&amp;SUBSTITUTE(I4,"'","''")&amp;"'" ),");")</f>
+        <v>1,'/VMS/common/welcome.html','Welcome page','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K4" s="6" t="str">
+        <f>IF($C$1="","", CONCATENATE($C$1,J4))</f>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (1,'/VMS/common/welcome.html','Welcome page','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="12">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="11">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6" t="str">
+        <f t="shared" ref="J5:J34" si="0">CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A5),"''",SUBSTITUTE(A5,"'", "''") ), "'"&amp;SUBSTITUTE(A5,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B5),"''",SUBSTITUTE(B5,"'","''") ), "'"&amp;SUBSTITUTE(B5,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C5),"''",SUBSTITUTE(C5,"'","''") ), "'"&amp;SUBSTITUTE(C5,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D5),"''",SUBSTITUTE(D5,"'","''") ), "'"&amp;SUBSTITUTE(D5,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E5),"''",SUBSTITUTE(E5,"'","''") ), "'"&amp;SUBSTITUTE(E5,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F5),"''",SUBSTITUTE(F5,"'","''") ), "'"&amp;SUBSTITUTE(F5,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G5),"''",SUBSTITUTE(G5,"'","''") ), "'"&amp;SUBSTITUTE(G5,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H5),"''",SUBSTITUTE(H5,"'","''") ), "'"&amp;SUBSTITUTE(H5,"'","''")&amp;"'" ),",",IF( ISTEXT($I$3), IF( ISBLANK(I5),"''",SUBSTITUTE(I5,"'","''") ), "'"&amp;SUBSTITUTE(I5,"'","''")&amp;"'" ),");")</f>
+        <v>2,'/VMS/admin/project/listProjects.html','Manage Projects',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K5" s="6" t="str">
+        <f t="shared" ref="K5:K34" si="1">IF($C$1="","", CONCATENATE($C$1,J5))</f>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (2,'/VMS/admin/project/listProjects.html','Manage Projects',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="11">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>3,'/VMS/admin/project/createProject.html','Create Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K6" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (3,'/VMS/admin/project/createProject.html','Create Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="12">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="11">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>4,'/VMS/admin/project/updateProject.html','Update Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K7" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (4,'/VMS/admin/project/updateProject.html','Update Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="6">
+        <v>2</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="11">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>5,'/VMS/admin/project/viewProject.html','View Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K8" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (5,'/VMS/admin/project/viewProject.html','View Project',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="12">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="11">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>6,'/VMS/admin/member/manageProjectMember.html','Manage Project Member',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K9" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (6,'/VMS/admin/member/manageProjectMember.html','Manage Project Member',2,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="6">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="6">
+        <v>3</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="11">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>7,'/VMS/admin/project/browseProjectFeedback.html','Review Project Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K10" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (7,'/VMS/admin/project/browseProjectFeedback.html','Review Project Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="12">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="6">
+        <v>3</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="11">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>8,'/VMS/admin/project/viewProjectFeedbackDetails.html','View Project Feeback Details',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K11" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (8,'/VMS/admin/project/viewProjectFeedbackDetails.html','View Project Feeback Details',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="6">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="6">
+        <v>3</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="11">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>9,'/VMS/admin/project/approveFb.html','Approve Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K12" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (9,'/VMS/admin/project/approveFb.html','Approve Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="12">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="6">
+        <v>3</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="11">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>10,'/VMS/admin/project/rejectFb.html','Reject Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K13" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (10,'/VMS/admin/project/rejectFb.html','Reject Feedback',3,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="12">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="6">
+        <v>4</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="11">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>11,'/VMS/admin/volunteer/browseProjectProposal.html','Browse Project Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K14" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (11,'/VMS/admin/volunteer/browseProjectProposal.html','Browse Project Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="6">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="6">
+        <v>4</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="11">
+        <v>1</v>
+      </c>
+      <c r="J15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>12,'/VMS/admin/volunteer/searchProjectProposal.html','Search Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K15" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (12,'/VMS/admin/volunteer/searchProjectProposal.html','Search Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="12">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="6">
+        <v>4</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="11">
+        <v>1</v>
+      </c>
+      <c r="J16" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>13,'/VMS/admin/volunteer/viewProjectProposalDetails.html','View Project Proposal Details',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K16" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (13,'/VMS/admin/volunteer/viewProjectProposalDetails.html','View Project Proposal Details',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="6">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="6">
+        <v>4</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="11">
+        <v>1</v>
+      </c>
+      <c r="J17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>14,'/VMS/admin/volunteer/reviewProposal.html','Review Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K17" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (14,'/VMS/admin/volunteer/reviewProposal.html','Review Proposal',4,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="20" customFormat="1">
+      <c r="A18" s="6">
+        <v>15</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="20">
+        <v>5</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="19">
+        <v>1</v>
+      </c>
+      <c r="J18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>15,'/VMS/admin/volunteer/proposeNewProject.html','Propose Project',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (15,'/VMS/admin/volunteer/proposeNewProject.html','Propose Project',5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="6">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="6">
+        <v>6</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="11">
+        <v>1</v>
+      </c>
+      <c r="J19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>16,'/VMS/admin/volunteer/browseProject.html','Browse Project (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K19" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (16,'/VMS/admin/volunteer/browseProject.html','Browse Project (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="12">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="6">
+        <v>6</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="11">
+        <v>1</v>
+      </c>
+      <c r="J20" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>17,'/VMS/admin/volunteer/searchProjects.html','Search Projects (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K20" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (17,'/VMS/admin/volunteer/searchProjects.html','Search Projects (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="6">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="6">
+        <v>6</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="11">
+        <v>1</v>
+      </c>
+      <c r="J21" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>18,'/VMS/admin/volunteer/viewProjectDetails.html','View Project Details (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K21" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (18,'/VMS/admin/volunteer/viewProjectDetails.html','View Project Details (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="6">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="6">
+        <v>6</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="11">
+        <v>1</v>
+      </c>
+      <c r="J22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>19,'/VMS/admin/volunteer/requestCertificate.html','Request Certificate (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K22" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (19,'/VMS/admin/volunteer/requestCertificate.html','Request Certificate (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="6">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="6">
+        <v>6</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" s="11">
+        <v>1</v>
+      </c>
+      <c r="J23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>20,'/VMS/admin/volunteer/postExperienceAndFb.html','Post Experience and Feedback (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K23" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (20,'/VMS/admin/volunteer/postExperienceAndFb.html','Post Experience and Feedback (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="12">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="6">
+        <v>6</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" s="11">
+        <v>1</v>
+      </c>
+      <c r="J24" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>21,'/VMS/admin/volunteer/raiseInterest.html','Raise Interest (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K24" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (21,'/VMS/admin/volunteer/raiseInterest.html','Raise Interest (Volunteer)',6,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="6">
+        <v>22</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="6">
+        <v>7</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="11">
+        <v>1</v>
+      </c>
+      <c r="J25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>22,'/VMS/common/welcome.html','My Project Interests',7,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K25" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (22,'/VMS/common/welcome.html','My Project Interests',7,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="12">
+        <v>23</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I26" s="19">
+        <v>1</v>
+      </c>
+      <c r="J26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>23,'/VMS/common/volunteer/registerVolunteer.html','Register Volunteer','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K26" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (23,'/VMS/common/volunteer/registerVolunteer.html','Register Volunteer','','SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="6">
+        <v>24</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="6">
+        <v>9</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27" s="11">
+        <v>1</v>
+      </c>
+      <c r="J27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>24,'/VMS/common/volunteer/updateVolunteer.html','My Profile',9,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K27" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (24,'/VMS/common/volunteer/updateVolunteer.html','My Profile',9,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="6">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="6">
+        <v>10</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="11">
+        <v>1</v>
+      </c>
+      <c r="J28" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>25,'/VMS/admin/user/changePassword.html','Change Password',10,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K28" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (25,'/VMS/admin/user/changePassword.html','Change Password',10,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="6">
+        <v>26</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="6">
+        <v>11</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="11">
+        <v>1</v>
+      </c>
+      <c r="J29" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>26,'/VMS/common/welcome.html','Forget Password',11,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K29" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (26,'/VMS/common/welcome.html','Forget Password',11,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="12">
+        <v>27</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="6">
+        <v>12</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" s="11">
+        <v>1</v>
+      </c>
+      <c r="J30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>27,'/VMS/common/welcome.html','Manage Volunteer',12,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K30" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (27,'/VMS/common/welcome.html','Manage Volunteer',12,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="6">
+        <v>28</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="6">
+        <v>13</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I31" s="11">
+        <v>1</v>
+      </c>
+      <c r="J31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>28,'/VMS/common/welcome.html','Manage Staff',13,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K31" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (28,'/VMS/common/welcome.html','Manage Staff',13,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="12">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="6">
+        <v>16</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" s="11">
+        <v>1</v>
+      </c>
+      <c r="J32" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>29,'/VMS/admin/reports/generateCertificate.html ','Generate Certificate',16,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K32" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (29,'/VMS/admin/reports/generateCertificate.html ','Generate Certificate',16,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="6">
+        <v>30</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="6">
+        <v>18</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" s="11">
+        <v>1</v>
+      </c>
+      <c r="J33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>30,'/VMS/common/welcome.html','Prepare Itinerary Plan',18,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K33" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (30,'/VMS/common/welcome.html','Prepare Itinerary Plan',18,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="6">
+        <v>31</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="6">
+        <v>19</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I34" s="11">
+        <v>1</v>
+      </c>
+      <c r="J34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>31,'/VMS/common/welcome.html','Review Intinerary Plan',19,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="K34" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO TB_PERMISSION (PERMI_ID, URI, PERMI_DESC, MENU_FUNC_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (31,'/VMS/common/welcome.html','Review Intinerary Plan',19,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="12"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="12"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="12"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="12"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="12"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="12"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="12"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="12"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="12"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="12"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="12"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="12"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="12"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="12"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="12"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="12"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="12"/>
+      <c r="B83" s="12"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="12"/>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="12"/>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="12"/>
+      <c r="B86" s="12"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="12"/>
+      <c r="B87" s="12"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="12"/>
+      <c r="B88" s="12"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="12"/>
+      <c r="B89" s="12"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="12"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="12"/>
+      <c r="B91" s="12"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="12"/>
+      <c r="B92" s="12"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="12"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="12"/>
+      <c r="B94" s="12"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="12"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="12"/>
+      <c r="B96" s="12"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="12"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="12"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="12"/>
+      <c r="B99" s="12"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="12"/>
+      <c r="B100" s="12"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="12"/>
+      <c r="B101" s="12"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="12"/>
+      <c r="B102" s="12"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="12"/>
+      <c r="B103" s="12"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="12"/>
+      <c r="B104" s="12"/>
+      <c r="C104" s="12"/>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="12"/>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="12"/>
+      <c r="B105" s="12"/>
+      <c r="C105" s="12"/>
+      <c r="D105" s="12"/>
+      <c r="E105" s="12"/>
+      <c r="F105" s="12"/>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="12"/>
+      <c r="B106" s="12"/>
+      <c r="C106" s="12"/>
+      <c r="D106" s="12"/>
+      <c r="E106" s="12"/>
+      <c r="F106" s="12"/>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="12"/>
+      <c r="B107" s="12"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
+      <c r="F107" s="12"/>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="12"/>
+      <c r="B108" s="12"/>
+      <c r="C108" s="12"/>
+      <c r="D108" s="12"/>
+      <c r="E108" s="12"/>
+      <c r="F108" s="12"/>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="12"/>
+      <c r="B109" s="12"/>
+      <c r="C109" s="12"/>
+      <c r="D109" s="12"/>
+      <c r="E109" s="12"/>
+      <c r="F109" s="12"/>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="12"/>
+      <c r="B110" s="12"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="12"/>
+      <c r="E110" s="12"/>
+      <c r="F110" s="12"/>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="12"/>
+      <c r="B111" s="12"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="12"/>
+      <c r="B112" s="12"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="12"/>
+      <c r="E112" s="12"/>
+      <c r="F112" s="12"/>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="12"/>
+      <c r="B113" s="12"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
+      <c r="F113" s="12"/>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="12"/>
+      <c r="B114" s="12"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="12"/>
+      <c r="B115" s="12"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="12"/>
+      <c r="E115" s="12"/>
+      <c r="F115" s="12"/>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="12"/>
+      <c r="B116" s="12"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
+      <c r="F116" s="12"/>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="12"/>
+      <c r="B117" s="12"/>
+      <c r="C117" s="12"/>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
+      <c r="F117" s="12"/>
+    </row>
+    <row r="118" spans="1:6" s="13" customFormat="1">
+      <c r="A118" s="12"/>
+      <c r="B118" s="12"/>
+      <c r="C118" s="12"/>
+      <c r="D118" s="12"/>
+      <c r="E118" s="12"/>
+      <c r="F118" s="12"/>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" s="12"/>
+      <c r="B119" s="12"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="12"/>
+      <c r="E119" s="12"/>
+      <c r="F119" s="12"/>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" s="12"/>
+      <c r="B120" s="12"/>
+      <c r="C120" s="12"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="12"/>
+      <c r="B121" s="12"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="12"/>
+      <c r="E121" s="12"/>
+      <c r="F121" s="12"/>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="12"/>
+      <c r="B122" s="12"/>
+      <c r="C122" s="12"/>
+      <c r="D122" s="12"/>
+      <c r="E122" s="12"/>
+      <c r="F122" s="12"/>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="12"/>
+      <c r="B123" s="12"/>
+      <c r="C123" s="12"/>
+      <c r="D123" s="12"/>
+      <c r="E123" s="12"/>
+      <c r="F123" s="12"/>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="12"/>
+      <c r="B124" s="12"/>
+      <c r="C124" s="12"/>
+      <c r="D124" s="12"/>
+      <c r="E124" s="12"/>
+      <c r="F124" s="12"/>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="12"/>
+      <c r="B125" s="12"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
+      <c r="F125" s="12"/>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="12"/>
+      <c r="B126" s="12"/>
+      <c r="C126" s="12"/>
+      <c r="D126" s="12"/>
+      <c r="E126" s="12"/>
+      <c r="F126" s="12"/>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="12"/>
+      <c r="B127" s="12"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
+      <c r="E127" s="12"/>
+      <c r="F127" s="12"/>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="12"/>
+      <c r="B128" s="12"/>
+      <c r="C128" s="12"/>
+      <c r="D128" s="12"/>
+      <c r="E128" s="12"/>
+      <c r="F128" s="12"/>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="12"/>
+      <c r="B129" s="12"/>
+      <c r="C129" s="12"/>
+      <c r="D129" s="12"/>
+      <c r="E129" s="12"/>
+      <c r="F129" s="12"/>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="12"/>
+      <c r="B130" s="12"/>
+      <c r="C130" s="12"/>
+      <c r="D130" s="12"/>
+      <c r="E130" s="12"/>
+      <c r="F130" s="12"/>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="12"/>
+      <c r="B131" s="12"/>
+      <c r="C131" s="12"/>
+      <c r="D131" s="12"/>
+      <c r="E131" s="12"/>
+      <c r="F131" s="12"/>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="12"/>
+      <c r="B132" s="12"/>
+      <c r="C132" s="12"/>
+      <c r="D132" s="12"/>
+      <c r="E132" s="12"/>
+      <c r="F132" s="12"/>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="12"/>
+      <c r="B133" s="12"/>
+      <c r="C133" s="12"/>
+      <c r="D133" s="12"/>
+      <c r="E133" s="12"/>
+      <c r="F133" s="12"/>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="12"/>
+      <c r="B134" s="12"/>
+      <c r="C134" s="12"/>
+      <c r="D134" s="12"/>
+      <c r="E134" s="12"/>
+      <c r="F134" s="12"/>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="12"/>
+      <c r="B135" s="12"/>
+      <c r="C135" s="12"/>
+      <c r="D135" s="12"/>
+      <c r="E135" s="12"/>
+      <c r="F135" s="12"/>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="12"/>
+      <c r="B136" s="12"/>
+      <c r="C136" s="12"/>
+      <c r="D136" s="12"/>
+      <c r="E136" s="12"/>
+      <c r="F136" s="12"/>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="12"/>
+      <c r="B137" s="12"/>
+      <c r="C137" s="12"/>
+      <c r="D137" s="12"/>
+      <c r="E137" s="12"/>
+      <c r="F137" s="12"/>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="12"/>
+      <c r="B138" s="12"/>
+      <c r="C138" s="12"/>
+      <c r="D138" s="12"/>
+      <c r="E138" s="12"/>
+      <c r="F138" s="12"/>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="12"/>
+      <c r="B139" s="12"/>
+      <c r="C139" s="12"/>
+      <c r="D139" s="12"/>
+      <c r="E139" s="12"/>
+      <c r="F139" s="12"/>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="12"/>
+      <c r="B140" s="12"/>
+      <c r="C140" s="12"/>
+      <c r="D140" s="12"/>
+      <c r="E140" s="12"/>
+      <c r="F140" s="12"/>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" s="12"/>
+      <c r="B141" s="12"/>
+      <c r="C141" s="12"/>
+      <c r="D141" s="12"/>
+      <c r="E141" s="12"/>
+      <c r="F141" s="12"/>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="12"/>
+      <c r="B142" s="12"/>
+      <c r="C142" s="12"/>
+      <c r="D142" s="12"/>
+      <c r="E142" s="12"/>
+      <c r="F142" s="12"/>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="12"/>
+      <c r="B143" s="12"/>
+      <c r="C143" s="12"/>
+      <c r="D143" s="12"/>
+      <c r="E143" s="12"/>
+      <c r="F143" s="12"/>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="12"/>
+      <c r="B144" s="12"/>
+      <c r="C144" s="12"/>
+      <c r="D144" s="12"/>
+      <c r="E144" s="12"/>
+      <c r="F144" s="12"/>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="12"/>
+      <c r="B145" s="12"/>
+      <c r="C145" s="12"/>
+      <c r="D145" s="12"/>
+      <c r="E145" s="12"/>
+      <c r="F145" s="12"/>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" s="12"/>
+      <c r="B146" s="12"/>
+      <c r="C146" s="12"/>
+      <c r="D146" s="12"/>
+      <c r="E146" s="12"/>
+      <c r="F146" s="12"/>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" s="12"/>
+      <c r="B147" s="12"/>
+      <c r="C147" s="12"/>
+      <c r="D147" s="12"/>
+      <c r="E147" s="12"/>
+      <c r="F147" s="12"/>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="12"/>
+      <c r="B148" s="12"/>
+      <c r="C148" s="12"/>
+      <c r="D148" s="12"/>
+      <c r="E148" s="12"/>
+      <c r="F148" s="12"/>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="12"/>
+      <c r="B149" s="12"/>
+      <c r="C149" s="12"/>
+      <c r="D149" s="12"/>
+      <c r="E149" s="12"/>
+      <c r="F149" s="12"/>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="12"/>
+      <c r="B150" s="12"/>
+      <c r="C150" s="12"/>
+      <c r="D150" s="12"/>
+      <c r="E150" s="12"/>
+      <c r="F150" s="12"/>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="12"/>
+      <c r="B151" s="12"/>
+      <c r="C151" s="12"/>
+      <c r="D151" s="12"/>
+      <c r="E151" s="12"/>
+      <c r="F151" s="12"/>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="12"/>
+      <c r="B152" s="12"/>
+      <c r="C152" s="12"/>
+      <c r="D152" s="12"/>
+      <c r="E152" s="12"/>
+      <c r="F152" s="12"/>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="12"/>
+      <c r="B153" s="12"/>
+      <c r="C153" s="12"/>
+      <c r="D153" s="12"/>
+      <c r="E153" s="12"/>
+      <c r="F153" s="12"/>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="12"/>
+      <c r="B154" s="12"/>
+      <c r="C154" s="12"/>
+      <c r="D154" s="12"/>
+      <c r="E154" s="12"/>
+      <c r="F154" s="12"/>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="12"/>
+      <c r="B155" s="12"/>
+      <c r="C155" s="12"/>
+      <c r="D155" s="12"/>
+      <c r="E155" s="12"/>
+      <c r="F155" s="12"/>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="12"/>
+      <c r="B156" s="12"/>
+      <c r="C156" s="12"/>
+      <c r="D156" s="12"/>
+      <c r="E156" s="12"/>
+      <c r="F156" s="12"/>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="12"/>
+      <c r="B157" s="12"/>
+      <c r="C157" s="12"/>
+      <c r="D157" s="12"/>
+      <c r="E157" s="12"/>
+      <c r="F157" s="12"/>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="12"/>
+      <c r="B158" s="12"/>
+      <c r="C158" s="12"/>
+      <c r="D158" s="12"/>
+      <c r="E158" s="12"/>
+      <c r="F158" s="12"/>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="12"/>
+      <c r="B159" s="12"/>
+      <c r="C159" s="12"/>
+      <c r="D159" s="12"/>
+      <c r="E159" s="12"/>
+      <c r="F159" s="12"/>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" s="12"/>
+      <c r="B160" s="12"/>
+      <c r="C160" s="12"/>
+      <c r="D160" s="12"/>
+      <c r="E160" s="12"/>
+      <c r="F160" s="12"/>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" s="12"/>
+      <c r="B161" s="12"/>
+      <c r="C161" s="12"/>
+      <c r="D161" s="12"/>
+      <c r="E161" s="12"/>
+      <c r="F161" s="12"/>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" s="12"/>
+      <c r="B162" s="12"/>
+      <c r="C162" s="12"/>
+      <c r="D162" s="12"/>
+      <c r="E162" s="12"/>
+      <c r="F162" s="12"/>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" s="12"/>
+      <c r="B163" s="12"/>
+      <c r="C163" s="12"/>
+      <c r="D163" s="12"/>
+      <c r="E163" s="12"/>
+      <c r="F163" s="12"/>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" s="12"/>
+      <c r="B164" s="12"/>
+      <c r="C164" s="12"/>
+      <c r="D164" s="12"/>
+      <c r="E164" s="12"/>
+      <c r="F164" s="12"/>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" s="12"/>
+      <c r="B165" s="12"/>
+      <c r="C165" s="12"/>
+      <c r="D165" s="12"/>
+      <c r="E165" s="12"/>
+      <c r="F165" s="12"/>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" s="12"/>
+      <c r="B166" s="12"/>
+      <c r="C166" s="12"/>
+      <c r="D166" s="12"/>
+      <c r="E166" s="12"/>
+      <c r="F166" s="12"/>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="A167" s="12"/>
+      <c r="B167" s="12"/>
+      <c r="C167" s="12"/>
+      <c r="D167" s="12"/>
+      <c r="E167" s="12"/>
+      <c r="F167" s="12"/>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" s="12"/>
+      <c r="B168" s="12"/>
+      <c r="C168" s="12"/>
+      <c r="D168" s="12"/>
+      <c r="E168" s="12"/>
+      <c r="F168" s="12"/>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" s="12"/>
+      <c r="B169" s="12"/>
+      <c r="C169" s="12"/>
+      <c r="D169" s="12"/>
+      <c r="E169" s="12"/>
+      <c r="F169" s="12"/>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="A170" s="12"/>
+      <c r="B170" s="12"/>
+      <c r="C170" s="12"/>
+      <c r="D170" s="12"/>
+      <c r="E170" s="12"/>
+      <c r="F170" s="12"/>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" s="12"/>
+      <c r="B171" s="12"/>
+      <c r="C171" s="12"/>
+      <c r="D171" s="12"/>
+      <c r="E171" s="12"/>
+      <c r="F171" s="12"/>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" s="12"/>
+      <c r="B172" s="12"/>
+      <c r="C172" s="12"/>
+      <c r="D172" s="12"/>
+      <c r="E172" s="12"/>
+      <c r="F172" s="12"/>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="A173" s="12"/>
+      <c r="B173" s="12"/>
+      <c r="C173" s="12"/>
+      <c r="D173" s="12"/>
+      <c r="E173" s="12"/>
+      <c r="F173" s="12"/>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" s="12"/>
+      <c r="B174" s="12"/>
+      <c r="C174" s="12"/>
+      <c r="D174" s="12"/>
+      <c r="E174" s="12"/>
+      <c r="F174" s="12"/>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" s="12"/>
+      <c r="B175" s="12"/>
+      <c r="C175" s="12"/>
+      <c r="D175" s="12"/>
+      <c r="E175" s="12"/>
+      <c r="F175" s="12"/>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" s="12"/>
+      <c r="B176" s="12"/>
+      <c r="C176" s="12"/>
+      <c r="D176" s="12"/>
+      <c r="E176" s="12"/>
+      <c r="F176" s="12"/>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" s="12"/>
+      <c r="B177" s="12"/>
+      <c r="C177" s="12"/>
+      <c r="D177" s="12"/>
+      <c r="E177" s="12"/>
+      <c r="F177" s="12"/>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" s="12"/>
+      <c r="B178" s="12"/>
+      <c r="C178" s="12"/>
+      <c r="D178" s="12"/>
+      <c r="E178" s="12"/>
+      <c r="F178" s="12"/>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" s="12"/>
+      <c r="B179" s="12"/>
+      <c r="C179" s="12"/>
+      <c r="D179" s="12"/>
+      <c r="E179" s="12"/>
+      <c r="F179" s="12"/>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" s="12"/>
+      <c r="B180" s="12"/>
+      <c r="C180" s="12"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="12"/>
+      <c r="F180" s="12"/>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" s="12"/>
+      <c r="B181" s="12"/>
+      <c r="C181" s="12"/>
+      <c r="D181" s="12"/>
+      <c r="E181" s="12"/>
+      <c r="F181" s="12"/>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" s="12"/>
+      <c r="B182" s="12"/>
+      <c r="C182" s="12"/>
+      <c r="D182" s="12"/>
+      <c r="E182" s="12"/>
+      <c r="F182" s="12"/>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" s="12"/>
+      <c r="B183" s="12"/>
+      <c r="C183" s="12"/>
+      <c r="D183" s="12"/>
+      <c r="E183" s="12"/>
+      <c r="F183" s="12"/>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" s="12"/>
+      <c r="B184" s="12"/>
+      <c r="C184" s="12"/>
+      <c r="D184" s="12"/>
+      <c r="E184" s="12"/>
+      <c r="F184" s="12"/>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" s="12"/>
+      <c r="B185" s="12"/>
+      <c r="C185" s="12"/>
+      <c r="D185" s="12"/>
+      <c r="E185" s="12"/>
+      <c r="F185" s="12"/>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" s="12"/>
+      <c r="B186" s="12"/>
+      <c r="C186" s="12"/>
+      <c r="D186" s="12"/>
+      <c r="E186" s="12"/>
+      <c r="F186" s="12"/>
+    </row>
+    <row r="187" spans="1:6">
+      <c r="A187" s="12"/>
+      <c r="B187" s="12"/>
+      <c r="C187" s="12"/>
+      <c r="D187" s="12"/>
+      <c r="E187" s="12"/>
+      <c r="F187" s="12"/>
+    </row>
+    <row r="188" spans="1:6">
+      <c r="A188" s="12"/>
+      <c r="B188" s="12"/>
+      <c r="C188" s="12"/>
+      <c r="D188" s="12"/>
+      <c r="E188" s="12"/>
+      <c r="F188" s="12"/>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" s="12"/>
+      <c r="B189" s="12"/>
+      <c r="C189" s="12"/>
+      <c r="D189" s="12"/>
+      <c r="E189" s="12"/>
+      <c r="F189" s="12"/>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" s="12"/>
+      <c r="B190" s="12"/>
+      <c r="C190" s="12"/>
+      <c r="D190" s="12"/>
+      <c r="E190" s="12"/>
+      <c r="F190" s="12"/>
+    </row>
+    <row r="191" spans="1:6">
+      <c r="A191" s="12"/>
+      <c r="B191" s="12"/>
+      <c r="C191" s="12"/>
+      <c r="D191" s="12"/>
+      <c r="E191" s="12"/>
+      <c r="F191" s="12"/>
+    </row>
+    <row r="192" spans="1:6">
+      <c r="A192" s="12"/>
+      <c r="B192" s="12"/>
+      <c r="C192" s="12"/>
+      <c r="D192" s="12"/>
+      <c r="E192" s="12"/>
+      <c r="F192" s="12"/>
+    </row>
+    <row r="193" spans="1:6">
+      <c r="A193" s="12"/>
+      <c r="B193" s="12"/>
+      <c r="C193" s="12"/>
+      <c r="D193" s="12"/>
+      <c r="E193" s="12"/>
+      <c r="F193" s="12"/>
+    </row>
+    <row r="194" spans="1:6">
+      <c r="A194" s="12"/>
+      <c r="B194" s="12"/>
+      <c r="C194" s="12"/>
+      <c r="D194" s="12"/>
+      <c r="E194" s="12"/>
+      <c r="F194" s="12"/>
+    </row>
+    <row r="195" spans="1:6">
+      <c r="A195" s="12"/>
+      <c r="B195" s="12"/>
+      <c r="C195" s="12"/>
+      <c r="D195" s="12"/>
+      <c r="E195" s="12"/>
+      <c r="F195" s="12"/>
+    </row>
+    <row r="196" spans="1:6">
+      <c r="A196" s="12"/>
+      <c r="B196" s="12"/>
+      <c r="C196" s="12"/>
+      <c r="D196" s="12"/>
+      <c r="E196" s="12"/>
+      <c r="F196" s="12"/>
+    </row>
+    <row r="197" spans="1:6">
+      <c r="A197" s="12"/>
+      <c r="B197" s="12"/>
+      <c r="C197" s="12"/>
+      <c r="D197" s="12"/>
+      <c r="E197" s="12"/>
+      <c r="F197" s="12"/>
+    </row>
+    <row r="198" spans="1:6">
+      <c r="A198" s="12"/>
+      <c r="B198" s="12"/>
+      <c r="C198" s="12"/>
+      <c r="D198" s="12"/>
+      <c r="E198" s="12"/>
+      <c r="F198" s="12"/>
+    </row>
+    <row r="199" spans="1:6">
+      <c r="A199" s="12"/>
+      <c r="B199" s="12"/>
+      <c r="C199" s="12"/>
+      <c r="D199" s="12"/>
+      <c r="E199" s="12"/>
+      <c r="F199" s="12"/>
+    </row>
+    <row r="200" spans="1:6">
+      <c r="A200" s="12"/>
+      <c r="B200" s="12"/>
+      <c r="C200" s="12"/>
+      <c r="D200" s="12"/>
+      <c r="E200" s="12"/>
+      <c r="F200" s="12"/>
+    </row>
+    <row r="201" spans="1:6">
+      <c r="A201" s="12"/>
+      <c r="B201" s="12"/>
+      <c r="C201" s="12"/>
+      <c r="D201" s="12"/>
+      <c r="E201" s="12"/>
+      <c r="F201" s="12"/>
+    </row>
+    <row r="202" spans="1:6">
+      <c r="A202" s="12"/>
+      <c r="B202" s="12"/>
+      <c r="C202" s="12"/>
+      <c r="D202" s="12"/>
+      <c r="E202" s="12"/>
+      <c r="F202" s="12"/>
+    </row>
+    <row r="203" spans="1:6">
+      <c r="A203" s="12"/>
+      <c r="B203" s="12"/>
+      <c r="C203" s="12"/>
+      <c r="D203" s="12"/>
+      <c r="E203" s="12"/>
+      <c r="F203" s="12"/>
+    </row>
+    <row r="204" spans="1:6">
+      <c r="A204" s="12"/>
+      <c r="B204" s="12"/>
+      <c r="C204" s="12"/>
+      <c r="D204" s="12"/>
+      <c r="E204" s="12"/>
+      <c r="F204" s="12"/>
+    </row>
+    <row r="205" spans="1:6">
+      <c r="A205" s="12"/>
+      <c r="B205" s="12"/>
+      <c r="C205" s="12"/>
+      <c r="D205" s="12"/>
+      <c r="E205" s="12"/>
+      <c r="F205" s="12"/>
+    </row>
+    <row r="206" spans="1:6">
+      <c r="A206" s="12"/>
+      <c r="B206" s="12"/>
+      <c r="C206" s="12"/>
+      <c r="D206" s="12"/>
+      <c r="E206" s="12"/>
+      <c r="F206" s="12"/>
+    </row>
+    <row r="207" spans="1:6">
+      <c r="A207" s="12"/>
+      <c r="B207" s="12"/>
+      <c r="C207" s="12"/>
+      <c r="D207" s="12"/>
+      <c r="E207" s="12"/>
+      <c r="F207" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8770,7 +11469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K180"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added permissions for Project Coordinator.
</commit_message>
<xml_diff>
--- a/src/doc/acl/acl_configuration.xlsx
+++ b/src/doc/acl/acl_configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380" tabRatio="573" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380" tabRatio="573" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="To be filled up by developer" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="133">
   <si>
     <t>Menu Name</t>
   </si>
@@ -566,7 +566,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="465">
+  <cellStyleXfs count="481">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1032,8 +1032,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1096,8 +1112,10 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="465">
+  <cellStyles count="481">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1330,6 +1348,14 @@
     <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1562,6 +1588,14 @@
     <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2544,7 +2578,7 @@
   <dimension ref="A1:K186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4456,9 +4490,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4779,7 +4813,7 @@
       <c r="B10" t="s">
         <v>107</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="28" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="6">
@@ -4816,7 +4850,7 @@
       <c r="B11" t="s">
         <v>108</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="28" t="s">
         <v>100</v>
       </c>
       <c r="D11" s="6">
@@ -4853,7 +4887,7 @@
       <c r="B12" t="s">
         <v>109</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="28" t="s">
         <v>101</v>
       </c>
       <c r="D12" s="6">
@@ -4890,7 +4924,7 @@
       <c r="B13" t="s">
         <v>110</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="28" t="s">
         <v>102</v>
       </c>
       <c r="D13" s="6">
@@ -4927,7 +4961,7 @@
       <c r="B14" t="s">
         <v>111</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="29" t="s">
         <v>103</v>
       </c>
       <c r="D14" s="6">
@@ -4964,7 +4998,7 @@
       <c r="B15" t="s">
         <v>112</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="28" t="s">
         <v>90</v>
       </c>
       <c r="D15" s="6">
@@ -5001,7 +5035,7 @@
       <c r="B16" t="s">
         <v>113</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="28" t="s">
         <v>91</v>
       </c>
       <c r="D16" s="6">
@@ -5038,7 +5072,7 @@
       <c r="B17" t="s">
         <v>122</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="28" t="s">
         <v>92</v>
       </c>
       <c r="D17" s="6">
@@ -5075,7 +5109,7 @@
       <c r="B18" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="27" t="s">
         <v>62</v>
       </c>
       <c r="D18" s="20">
@@ -5112,7 +5146,7 @@
       <c r="B19" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="29" t="s">
         <v>49</v>
       </c>
       <c r="D19" s="6">
@@ -5260,7 +5294,7 @@
       <c r="B23" t="s">
         <v>118</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="29" t="s">
         <v>53</v>
       </c>
       <c r="D23" s="6">
@@ -5297,7 +5331,7 @@
       <c r="B24" t="s">
         <v>119</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="29" t="s">
         <v>51</v>
       </c>
       <c r="D24" s="6">
@@ -5371,7 +5405,7 @@
       <c r="B26" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="27" t="s">
         <v>70</v>
       </c>
       <c r="E26" s="19" t="s">
@@ -5405,7 +5439,7 @@
       <c r="B27" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="29" t="s">
         <v>26</v>
       </c>
       <c r="D27" s="6">
@@ -5516,7 +5550,7 @@
       <c r="B30" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="29" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="6">
@@ -5553,7 +5587,7 @@
       <c r="B31" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="29" t="s">
         <v>29</v>
       </c>
       <c r="D31" s="6">
@@ -5627,7 +5661,7 @@
       <c r="B33" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="29" t="s">
         <v>33</v>
       </c>
       <c r="D33" s="6">
@@ -5664,7 +5698,7 @@
       <c r="B34" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="29" t="s">
         <v>34</v>
       </c>
       <c r="D34" s="6">
@@ -5701,7 +5735,7 @@
       <c r="B35" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="27" t="s">
         <v>128</v>
       </c>
       <c r="D35" s="20">
@@ -5738,7 +5772,7 @@
       <c r="B36" t="s">
         <v>131</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="28" t="s">
         <v>132</v>
       </c>
       <c r="D36" s="6">
@@ -9762,7 +9796,7 @@
   <dimension ref="A1:K190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21:J22"/>
+      <selection activeCell="J23" sqref="J23:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10498,46 +10532,208 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="A23" s="12">
+        <v>20</v>
+      </c>
+      <c r="B23" s="12">
+        <v>20</v>
+      </c>
+      <c r="C23" s="12">
+        <v>5</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="11">
+        <v>2</v>
+      </c>
+      <c r="I23" s="6" t="str">
+        <f t="shared" ref="I23:I28" si="4">CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A23),"''",SUBSTITUTE(A23,"'", "''") ), "'"&amp;SUBSTITUTE(A23,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B23),"''",SUBSTITUTE(B23,"'","''") ), "'"&amp;SUBSTITUTE(B23,"'","''")&amp;"'" ),",",IF( ISTEXT($C$3), IF( ISBLANK(C23),"''",SUBSTITUTE(C23,"'","''") ), "'"&amp;SUBSTITUTE(C23,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D23),"''",SUBSTITUTE(D23,"'","''") ), "'"&amp;SUBSTITUTE(D23,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E23),"''",SUBSTITUTE(E23,"'","''") ), "'"&amp;SUBSTITUTE(E23,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F23),"''",SUBSTITUTE(F23,"'","''") ), "'"&amp;SUBSTITUTE(F23,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G23),"''",SUBSTITUTE(G23,"'","''") ), "'"&amp;SUBSTITUTE(G23,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H23),"''",SUBSTITUTE(H23,"'","''") ), "'"&amp;SUBSTITUTE(H23,"'","''")&amp;"'" ),");")</f>
+        <v>20,20,5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,2);</v>
+      </c>
+      <c r="J23" s="6" t="str">
+        <f t="shared" ref="J23:J28" si="5">IF($C$1="","", CONCATENATE($C$1,I23))</f>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (20,20,5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,2);</v>
+      </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
+      <c r="A24" s="12">
+        <v>21</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+      <c r="C24" s="12">
+        <v>5</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" s="11">
+        <v>3</v>
+      </c>
+      <c r="I24" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>21,1,5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,3);</v>
+      </c>
+      <c r="J24" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (21,1,5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,3);</v>
+      </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
+      <c r="A25" s="12">
+        <v>22</v>
+      </c>
+      <c r="B25" s="12">
+        <v>4</v>
+      </c>
+      <c r="C25" s="12">
+        <v>5</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" s="11">
+        <v>4</v>
+      </c>
+      <c r="I25" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>22,4,5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,4);</v>
+      </c>
+      <c r="J25" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (22,4,5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,4);</v>
+      </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="A26" s="12">
+        <v>23</v>
+      </c>
+      <c r="B26" s="12">
+        <v>6</v>
+      </c>
+      <c r="C26" s="12">
+        <v>5</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="11">
+        <v>5</v>
+      </c>
+      <c r="I26" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>23,6,5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,5);</v>
+      </c>
+      <c r="J26" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (23,6,5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,5);</v>
+      </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
+      <c r="A27" s="12">
+        <v>24</v>
+      </c>
+      <c r="B27" s="12">
+        <v>8</v>
+      </c>
+      <c r="C27" s="12">
+        <v>5</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="11">
+        <v>6</v>
+      </c>
+      <c r="I27" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>24,8,5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,6);</v>
+      </c>
+      <c r="J27" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (24,8,5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,6);</v>
+      </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
+      <c r="A28" s="12">
+        <v>25</v>
+      </c>
+      <c r="B28" s="12">
+        <v>9</v>
+      </c>
+      <c r="C28" s="12">
+        <v>5</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H28" s="11">
+        <v>7</v>
+      </c>
+      <c r="I28" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>25,9,5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,7);</v>
+      </c>
+      <c r="J28" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO TB_ROLE_FUNCTION (ROLE_FUNC_ID, MENU_FUNC_ID, ROLE_ID, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (25,9,5,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,7);</v>
+      </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="12"/>
@@ -11689,7 +11885,7 @@
   <dimension ref="A1:K180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11779,7 +11975,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="6">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>13</v>
@@ -11798,11 +11994,11 @@
       </c>
       <c r="I4" s="6" t="str">
         <f>CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A4),"''",SUBSTITUTE(A4,"'", "''") ), "'"&amp;SUBSTITUTE(A4,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B4),"''",SUBSTITUTE(B4,"'","''") ), "'"&amp;SUBSTITUTE(B4,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D4),"''",SUBSTITUTE(D4,"'","''") ), "'"&amp;SUBSTITUTE(D4,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E4),"''",SUBSTITUTE(E4,"'","''") ), "'"&amp;SUBSTITUTE(E4,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F4),"''",SUBSTITUTE(F4,"'","''") ), "'"&amp;SUBSTITUTE(F4,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G4),"''",SUBSTITUTE(G4,"'","''") ), "'"&amp;SUBSTITUTE(G4,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H4),"''",SUBSTITUTE(H4,"'","''") ), "'"&amp;SUBSTITUTE(H4,"'","''")&amp;"'" ),");")</f>
-        <v>1,38,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>1,47,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J4" s="6" t="str">
         <f>IF($C$1="","", CONCATENATE($C$1,I4))</f>
-        <v>INSERT INTO TB_ROLE (ROLE_ID, ROLE_CD, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (1,38,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE (ROLE_ID, ROLE_CD, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (1,47,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -11810,7 +12006,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="12">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="11" t="s">
@@ -11830,11 +12026,11 @@
       </c>
       <c r="I5" s="6" t="str">
         <f t="shared" ref="I5:I7" si="0">CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A5),"''",SUBSTITUTE(A5,"'", "''") ), "'"&amp;SUBSTITUTE(A5,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B5),"''",SUBSTITUTE(B5,"'","''") ), "'"&amp;SUBSTITUTE(B5,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D5),"''",SUBSTITUTE(D5,"'","''") ), "'"&amp;SUBSTITUTE(D5,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E5),"''",SUBSTITUTE(E5,"'","''") ), "'"&amp;SUBSTITUTE(E5,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F5),"''",SUBSTITUTE(F5,"'","''") ), "'"&amp;SUBSTITUTE(F5,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G5),"''",SUBSTITUTE(G5,"'","''") ), "'"&amp;SUBSTITUTE(G5,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H5),"''",SUBSTITUTE(H5,"'","''") ), "'"&amp;SUBSTITUTE(H5,"'","''")&amp;"'" ),");")</f>
-        <v>2,36,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>2,34,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J5" s="6" t="str">
         <f t="shared" ref="J5:J7" si="1">IF($C$1="","", CONCATENATE($C$1,I5))</f>
-        <v>INSERT INTO TB_ROLE (ROLE_ID, ROLE_CD, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (2,36,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE (ROLE_ID, ROLE_CD, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (2,34,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -11842,7 +12038,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="12">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="11" t="s">
@@ -11862,11 +12058,11 @@
       </c>
       <c r="I6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>3,34,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>3,36,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J6" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE (ROLE_ID, ROLE_CD, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (3,34,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE (ROLE_ID, ROLE_CD, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (3,36,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -11874,7 +12070,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="12">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="11" t="s">
@@ -11894,19 +12090,44 @@
       </c>
       <c r="I7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>4,36,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>4,34,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
       <c r="J7" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO TB_ROLE (ROLE_ID, ROLE_CD, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (4,36,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+        <v>INSERT INTO TB_ROLE (ROLE_ID, ROLE_CD, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (4,34,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="12">
+        <v>5</v>
+      </c>
+      <c r="B8" s="12">
+        <v>38</v>
+      </c>
       <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="D8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="11">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6" t="str">
+        <f t="shared" ref="I8" si="2">CONCATENATE(IF( ISTEXT($A$3), IF( ISBLANK(A8),"''",SUBSTITUTE(A8,"'", "''") ), "'"&amp;SUBSTITUTE(A8,"'","''")&amp;"'" ),",",IF( ISTEXT($B$3), IF( ISBLANK(B8),"''",SUBSTITUTE(B8,"'","''") ), "'"&amp;SUBSTITUTE(B8,"'","''")&amp;"'" ),",",IF( ISTEXT($D$3), IF( ISBLANK(D8),"''",SUBSTITUTE(D8,"'","''") ), "'"&amp;SUBSTITUTE(D8,"'","''")&amp;"'" ),",",IF( ISTEXT($E$3), IF( ISBLANK(E8),"''",SUBSTITUTE(E8,"'","''") ), "'"&amp;SUBSTITUTE(E8,"'","''")&amp;"'" ),",",IF( ISTEXT($F$3), IF( ISBLANK(F8),"''",SUBSTITUTE(F8,"'","''") ), "'"&amp;SUBSTITUTE(F8,"'","''")&amp;"'" ),",",IF( ISTEXT($G$3), IF( ISBLANK(G8),"''",SUBSTITUTE(G8,"'","''") ), "'"&amp;SUBSTITUTE(G8,"'","''")&amp;"'" ),",",IF( ISTEXT($H$3), IF( ISBLANK(H8),"''",SUBSTITUTE(H8,"'","''") ), "'"&amp;SUBSTITUTE(H8,"'","''")&amp;"'" ),");")</f>
+        <v>5,38,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
+      <c r="J8" s="6" t="str">
+        <f t="shared" ref="J8" si="3">IF($C$1="","", CONCATENATE($C$1,I8))</f>
+        <v>INSERT INTO TB_ROLE (ROLE_ID, ROLE_CD, CREATED_BY, CREATED_DTE, UPD_BY, UPD_DTE, VERSION) VALUES (5,38,'SYSTEM',CURRENT_TIMESTAMP,'SYSTEM',CURRENT_TIMESTAMP,1);</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="12"/>

</xml_diff>